<commit_message>
updated agenda-pdf and -xlsx files
</commit_message>
<xml_diff>
--- a/ui5con/downloads/ui5con_2017_agenda.xlsx
+++ b/ui5con/downloads/ui5con_2017_agenda.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D050079\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D038767\Documents\UI5con\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="0" windowWidth="23040" windowHeight="7920"/>
+    <workbookView xWindow="1392" yWindow="0" windowWidth="23040" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda UI5con@SAP" sheetId="1" r:id="rId1"/>
@@ -133,9 +133,6 @@
     <t>Aparna Narayanaswamy</t>
   </si>
   <si>
-    <t>Michael Graf</t>
-  </si>
-  <si>
     <t>HP Seitz</t>
   </si>
   <si>
@@ -822,29 +819,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>EMBEDDED ANALYTICS WITH CHARTS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Pia Kinkel, Christoph Laux, Bohdan Pukalskyi 
-11:00 - 12:00</t>
-    </r>
-  </si>
-  <si>
     <t>Advanced Charting Controls Coming to UI5</t>
   </si>
   <si>
@@ -1110,29 +1084,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>UI5 CONTROLS FOR DOCUMENT HANDLING</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Pia Kinkel, Christoph Laux
-10:00 - 11:00</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>DEVELOPING CUSTOM ESLINT RULES</t>
     </r>
     <r>
@@ -1248,29 +1199,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>COLLABORATORS WANTED FOR UI5LAB - A CUSTOM UI5 REPO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Michael Graf, Emmanuele Ricci
-14:20 - 14:40                                          </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve">MIXED REALITY WITH OPENUI5
 </t>
     </r>
@@ -1882,13 +1810,88 @@
       </rPr>
       <t>AGENDA 2017</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>COLLABORATORS WANTED FOR UI5LAB - A CUSTOM UI5 REPO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Michael Graf, Emanuele Ricci
+14:20 - 14:40                                          </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>UI5 CONTROLS FOR DOCUMENT HANDLING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Pia Kinkel, Christoph Laux
+10:40 - 11:20</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>EMBEDDED ANALYTICS WITH CHARTS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Pia Kinkel, Christoph Laux, Bohdan Pukalskyi 
+11:20 - 12:00</t>
+    </r>
+  </si>
+  <si>
+    <t>Michael Graf, Emanuele Ricci</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###,000"/>
+  </numFmts>
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1988,8 +1991,91 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF1F497D"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF1F497D"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF00CC00"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF33CC33"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF9900"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF1F497D"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF1F497D"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2002,8 +2088,110 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBE5F1"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1F5FB"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9EFF7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6F9C1"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFABEDA5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF94D88F"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFDBF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFB8C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF843"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF988C"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6758"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBE5F1"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7CFE8"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC3D6EB"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBE5F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -2063,10 +2251,187 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="3" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="3" tint="0.59996337778862885"/>
+      </left>
+      <right style="thin">
+        <color theme="3" tint="0.59996337778862885"/>
+      </right>
+      <top style="thin">
+        <color theme="3" tint="0.59996337778862885"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3" tint="0.59996337778862885"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right style="hair">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="8" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="12" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="15" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="5" borderId="7" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="6" borderId="6" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="6" borderId="7" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2184,6 +2549,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2226,11 +2592,46 @@
     <xf numFmtId="20" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="38">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="SAPBorder" xfId="20"/>
+    <cellStyle name="SAPDataCell" xfId="3"/>
+    <cellStyle name="SAPDataTotalCell" xfId="4"/>
+    <cellStyle name="SAPDimensionCell" xfId="2"/>
+    <cellStyle name="SAPEditableDataCell" xfId="5"/>
+    <cellStyle name="SAPEditableDataTotalCell" xfId="8"/>
+    <cellStyle name="SAPEmphasized" xfId="28"/>
+    <cellStyle name="SAPEmphasizedEditableDataCell" xfId="30"/>
+    <cellStyle name="SAPEmphasizedEditableDataTotalCell" xfId="31"/>
+    <cellStyle name="SAPEmphasizedLockedDataCell" xfId="34"/>
+    <cellStyle name="SAPEmphasizedLockedDataTotalCell" xfId="35"/>
+    <cellStyle name="SAPEmphasizedReadonlyDataCell" xfId="32"/>
+    <cellStyle name="SAPEmphasizedReadonlyDataTotalCell" xfId="33"/>
+    <cellStyle name="SAPEmphasizedTotal" xfId="29"/>
+    <cellStyle name="SAPExceptionLevel1" xfId="11"/>
+    <cellStyle name="SAPExceptionLevel2" xfId="12"/>
+    <cellStyle name="SAPExceptionLevel3" xfId="13"/>
+    <cellStyle name="SAPExceptionLevel4" xfId="14"/>
+    <cellStyle name="SAPExceptionLevel5" xfId="15"/>
+    <cellStyle name="SAPExceptionLevel6" xfId="16"/>
+    <cellStyle name="SAPExceptionLevel7" xfId="17"/>
+    <cellStyle name="SAPExceptionLevel8" xfId="18"/>
+    <cellStyle name="SAPExceptionLevel9" xfId="19"/>
+    <cellStyle name="SAPFormula" xfId="37"/>
+    <cellStyle name="SAPHierarchyCell0" xfId="23"/>
+    <cellStyle name="SAPHierarchyCell1" xfId="24"/>
+    <cellStyle name="SAPHierarchyCell2" xfId="25"/>
+    <cellStyle name="SAPHierarchyCell3" xfId="26"/>
+    <cellStyle name="SAPHierarchyCell4" xfId="27"/>
+    <cellStyle name="SAPLockedDataCell" xfId="7"/>
+    <cellStyle name="SAPLockedDataTotalCell" xfId="10"/>
+    <cellStyle name="SAPMemberCell" xfId="21"/>
+    <cellStyle name="SAPMemberTotalCell" xfId="22"/>
+    <cellStyle name="SAPMessageText" xfId="36"/>
+    <cellStyle name="SAPReadonlyDataCell" xfId="6"/>
+    <cellStyle name="SAPReadonlyDataTotalCell" xfId="9"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2554,34 +2955,34 @@
   <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="4"/>
-    <col min="2" max="2" width="1.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="2.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="2.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="2.140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="2.140625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="35.7109375" style="4" customWidth="1"/>
-    <col min="12" max="12" width="2.140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="35.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="2.140625" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="1.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="2.109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="2.109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="2.109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="2.109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="35.6640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="2.109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="35.6640625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="2.109375" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.3">
-      <c r="C1" s="55" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="3" customFormat="1" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="24" x14ac:dyDescent="0.4">
+      <c r="C1" s="41" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="3" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
@@ -2612,47 +3013,47 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
         <v>0.39583333333333331</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="50" t="s">
-        <v>137</v>
-      </c>
       <c r="F3" s="22"/>
-      <c r="G3" s="48"/>
+      <c r="G3" s="49"/>
       <c r="H3" s="17"/>
-      <c r="I3" s="52"/>
+      <c r="I3" s="53"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="52"/>
+      <c r="K3" s="53"/>
       <c r="L3" s="22"/>
-      <c r="M3" s="48"/>
+      <c r="M3" s="49"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="51"/>
+      <c r="C4" s="52"/>
       <c r="D4" s="17"/>
-      <c r="E4" s="51"/>
+      <c r="E4" s="52"/>
       <c r="F4" s="17"/>
-      <c r="G4" s="49"/>
+      <c r="G4" s="50"/>
       <c r="H4" s="17"/>
-      <c r="I4" s="53"/>
+      <c r="I4" s="54"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="53"/>
+      <c r="K4" s="54"/>
       <c r="L4" s="17"/>
-      <c r="M4" s="49"/>
+      <c r="M4" s="50"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21"/>
       <c r="B5" s="5"/>
       <c r="C5" s="16"/>
@@ -2669,66 +3070,64 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37">
         <v>0.41666666666666669</v>
       </c>
       <c r="B6" s="31"/>
-      <c r="C6" s="41" t="s">
-        <v>139</v>
+      <c r="C6" s="42" t="s">
+        <v>138</v>
       </c>
       <c r="D6" s="13"/>
-      <c r="E6" s="41" t="s">
-        <v>138</v>
+      <c r="E6" s="42" t="s">
+        <v>137</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
-      <c r="I6" s="44"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="13"/>
-      <c r="K6" s="44"/>
+      <c r="K6" s="45"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="37"/>
       <c r="B7" s="31"/>
-      <c r="C7" s="42"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="42"/>
+      <c r="E7" s="43"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="44"/>
+      <c r="I7" s="45"/>
       <c r="J7" s="13"/>
-      <c r="K7" s="44"/>
+      <c r="K7" s="45"/>
       <c r="L7" s="13"/>
-      <c r="M7" s="41" t="s">
-        <v>167</v>
-      </c>
+      <c r="M7" s="6"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="37"/>
       <c r="B8" s="31"/>
-      <c r="C8" s="43"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="43"/>
+      <c r="E8" s="44"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="44"/>
+      <c r="I8" s="45"/>
       <c r="J8" s="13"/>
-      <c r="K8" s="44"/>
+      <c r="K8" s="45"/>
       <c r="L8" s="13"/>
-      <c r="M8" s="42"/>
+      <c r="M8" s="6"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37">
         <v>0.4375</v>
       </c>
@@ -2743,93 +3142,93 @@
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
-      <c r="M9" s="42"/>
+      <c r="M9" s="6"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37"/>
       <c r="B10" s="31"/>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="46" t="s">
         <v>158</v>
-      </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="45" t="s">
-        <v>159</v>
-      </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="45" t="s">
-        <v>160</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="44"/>
+      <c r="J10" s="45"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="42"/>
+      <c r="M10" s="42" t="s">
+        <v>197</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="38">
         <v>0.45833333333333331</v>
       </c>
       <c r="B11" s="31"/>
-      <c r="C11" s="46"/>
+      <c r="C11" s="47"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="46"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="46"/>
+      <c r="G11" s="47"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="45" t="s">
-        <v>161</v>
-      </c>
-      <c r="J11" s="44"/>
-      <c r="K11" s="45" t="s">
-        <v>162</v>
+      <c r="I11" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46" t="s">
+        <v>160</v>
       </c>
       <c r="L11" s="13"/>
       <c r="M11" s="43"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" s="26" customFormat="1" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="26" customFormat="1" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="39"/>
       <c r="B12" s="31"/>
-      <c r="C12" s="46"/>
+      <c r="C12" s="47"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="46"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="46"/>
+      <c r="G12" s="47"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="46"/>
+      <c r="I12" s="47"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="46"/>
+      <c r="K12" s="47"/>
       <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
+      <c r="M12" s="43"/>
       <c r="N12" s="25"/>
       <c r="O12" s="25"/>
     </row>
-    <row r="13" spans="1:15" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37"/>
       <c r="B13" s="31"/>
-      <c r="C13" s="47"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="47"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="47"/>
+      <c r="G13" s="48"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="46"/>
+      <c r="I13" s="47"/>
       <c r="J13" s="13"/>
-      <c r="K13" s="46"/>
+      <c r="K13" s="47"/>
       <c r="L13" s="13"/>
-      <c r="M13" s="41" t="s">
-        <v>151</v>
-      </c>
+      <c r="M13" s="44"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37"/>
       <c r="B14" s="31"/>
       <c r="C14" s="13"/>
@@ -2838,25 +3237,27 @@
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="47"/>
+      <c r="I14" s="48"/>
       <c r="J14" s="13"/>
-      <c r="K14" s="47"/>
+      <c r="K14" s="48"/>
       <c r="L14" s="13"/>
-      <c r="M14" s="42"/>
+      <c r="M14" s="42" t="s">
+        <v>198</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37">
         <v>0.47916666666666669</v>
       </c>
       <c r="B15" s="31"/>
-      <c r="C15" s="45" t="s">
-        <v>170</v>
+      <c r="C15" s="46" t="s">
+        <v>167</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="E15" s="45" t="s">
-        <v>169</v>
+      <c r="E15" s="46" t="s">
+        <v>166</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
@@ -2865,167 +3266,167 @@
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="42"/>
+      <c r="M15" s="43"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37"/>
       <c r="B16" s="31"/>
-      <c r="C16" s="46"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="46"/>
+      <c r="E16" s="47"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
-      <c r="I16" s="45" t="s">
-        <v>163</v>
+      <c r="I16" s="46" t="s">
+        <v>161</v>
       </c>
       <c r="J16" s="13"/>
-      <c r="K16" s="45" t="s">
-        <v>166</v>
+      <c r="K16" s="46" t="s">
+        <v>164</v>
       </c>
       <c r="L16" s="13"/>
-      <c r="M16" s="42"/>
+      <c r="M16" s="43"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37"/>
       <c r="B17" s="31"/>
-      <c r="C17" s="46"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="13"/>
-      <c r="E17" s="46"/>
+      <c r="E17" s="47"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="45" t="s">
-        <v>144</v>
+      <c r="G17" s="46" t="s">
+        <v>143</v>
       </c>
       <c r="H17" s="13"/>
-      <c r="I17" s="46"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="13"/>
-      <c r="K17" s="46"/>
+      <c r="K17" s="47"/>
       <c r="L17" s="13"/>
       <c r="M17" s="43"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="37">
         <v>0.5</v>
       </c>
       <c r="B18" s="31"/>
-      <c r="C18" s="47"/>
+      <c r="C18" s="48"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="47"/>
+      <c r="E18" s="48"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="46"/>
+      <c r="G18" s="47"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="46"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="47"/>
       <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
+      <c r="M18" s="44"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37"/>
       <c r="B19" s="31"/>
       <c r="C19" s="32"/>
       <c r="D19" s="13"/>
       <c r="E19" s="32"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="46"/>
+      <c r="G19" s="47"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="47"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="48"/>
       <c r="L19" s="13"/>
-      <c r="M19" s="41" t="s">
-        <v>145</v>
+      <c r="M19" s="42" t="s">
+        <v>144</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37"/>
       <c r="B20" s="31"/>
-      <c r="C20" s="45" t="s">
-        <v>171</v>
+      <c r="C20" s="46" t="s">
+        <v>168</v>
       </c>
       <c r="D20" s="13"/>
-      <c r="E20" s="45" t="s">
-        <v>168</v>
+      <c r="E20" s="46" t="s">
+        <v>165</v>
       </c>
       <c r="F20" s="13"/>
-      <c r="G20" s="46"/>
+      <c r="G20" s="47"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
-      <c r="M20" s="42"/>
+      <c r="M20" s="43"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37">
         <v>0.52083333333333337</v>
       </c>
       <c r="B21" s="31"/>
-      <c r="C21" s="46"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="46"/>
+      <c r="E21" s="47"/>
       <c r="F21" s="13"/>
-      <c r="G21" s="46"/>
+      <c r="G21" s="47"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="J21" s="44"/>
-      <c r="K21" s="45" t="s">
-        <v>165</v>
+      <c r="I21" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="J21" s="45"/>
+      <c r="K21" s="46" t="s">
+        <v>163</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="42"/>
+      <c r="M21" s="43"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37"/>
       <c r="B22" s="31"/>
-      <c r="C22" s="46"/>
+      <c r="C22" s="47"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="46"/>
+      <c r="E22" s="47"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="47"/>
+      <c r="G22" s="48"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="46"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="47"/>
       <c r="L22" s="13"/>
-      <c r="M22" s="43"/>
+      <c r="M22" s="44"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="37"/>
       <c r="B23" s="31"/>
-      <c r="C23" s="47"/>
+      <c r="C23" s="48"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="47"/>
+      <c r="E23" s="48"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
-      <c r="I23" s="46"/>
+      <c r="I23" s="47"/>
       <c r="J23" s="13"/>
-      <c r="K23" s="46"/>
+      <c r="K23" s="47"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="37">
         <v>0.54166666666666663</v>
       </c>
@@ -3036,17 +3437,17 @@
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="46"/>
+      <c r="I24" s="47"/>
       <c r="J24" s="13"/>
-      <c r="K24" s="46"/>
+      <c r="K24" s="47"/>
       <c r="L24" s="13"/>
-      <c r="M24" s="41" t="s">
-        <v>150</v>
+      <c r="M24" s="42" t="s">
+        <v>149</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
       <c r="B25" s="31"/>
       <c r="C25" s="13"/>
@@ -3055,15 +3456,15 @@
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
-      <c r="I25" s="47"/>
+      <c r="I25" s="48"/>
       <c r="J25" s="13"/>
-      <c r="K25" s="47"/>
+      <c r="K25" s="48"/>
       <c r="L25" s="13"/>
-      <c r="M25" s="42"/>
+      <c r="M25" s="43"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37"/>
       <c r="B26" s="31"/>
       <c r="C26" s="13"/>
@@ -3076,19 +3477,19 @@
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
-      <c r="M26" s="42"/>
+      <c r="M26" s="43"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37">
         <v>0.5625</v>
       </c>
       <c r="B27" s="31"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
-      <c r="E27" s="45" t="s">
-        <v>178</v>
+      <c r="E27" s="46" t="s">
+        <v>174</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
@@ -3097,56 +3498,56 @@
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
-      <c r="M27" s="42"/>
+      <c r="M27" s="43"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
       <c r="B28" s="31"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
-      <c r="E28" s="46"/>
+      <c r="E28" s="47"/>
       <c r="F28" s="13"/>
-      <c r="G28" s="45" t="s">
-        <v>184</v>
+      <c r="G28" s="46" t="s">
+        <v>180</v>
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
-      <c r="M28" s="42"/>
+      <c r="M28" s="43"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="37"/>
       <c r="B29" s="31"/>
-      <c r="C29" s="45" t="s">
-        <v>172</v>
+      <c r="C29" s="46" t="s">
+        <v>169</v>
       </c>
       <c r="D29" s="13"/>
-      <c r="E29" s="46"/>
+      <c r="E29" s="47"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="46"/>
+      <c r="G29" s="47"/>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
-      <c r="M29" s="43"/>
+      <c r="M29" s="44"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="37"/>
       <c r="B30" s="31"/>
-      <c r="C30" s="46"/>
+      <c r="C30" s="47"/>
       <c r="D30" s="13"/>
-      <c r="E30" s="46"/>
+      <c r="E30" s="47"/>
       <c r="F30" s="13"/>
-      <c r="G30" s="46"/>
+      <c r="G30" s="47"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
@@ -3156,89 +3557,89 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="37">
         <v>0.58333333333333337</v>
       </c>
       <c r="B31" s="31"/>
-      <c r="C31" s="47"/>
+      <c r="C31" s="48"/>
       <c r="D31" s="13"/>
-      <c r="E31" s="47"/>
+      <c r="E31" s="48"/>
       <c r="F31" s="13"/>
-      <c r="G31" s="46"/>
+      <c r="G31" s="47"/>
       <c r="H31" s="13"/>
-      <c r="I31" s="45" t="s">
+      <c r="I31" s="46" t="s">
+        <v>183</v>
+      </c>
+      <c r="J31" s="13"/>
+      <c r="K31" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="J31" s="13"/>
-      <c r="K31" s="45" t="s">
-        <v>191</v>
-      </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="41" t="s">
-        <v>149</v>
+      <c r="M31" s="42" t="s">
+        <v>148</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="37"/>
       <c r="B32" s="34"/>
       <c r="C32" s="33"/>
       <c r="D32" s="13"/>
       <c r="E32" s="33"/>
       <c r="F32" s="13"/>
-      <c r="G32" s="46"/>
+      <c r="G32" s="47"/>
       <c r="H32" s="13"/>
-      <c r="I32" s="46"/>
+      <c r="I32" s="47"/>
       <c r="J32" s="13"/>
-      <c r="K32" s="46"/>
+      <c r="K32" s="47"/>
       <c r="L32" s="13"/>
-      <c r="M32" s="42"/>
+      <c r="M32" s="43"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="1:15" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="37"/>
       <c r="B33" s="34"/>
-      <c r="C33" s="45" t="s">
-        <v>173</v>
+      <c r="C33" s="46" t="s">
+        <v>196</v>
       </c>
       <c r="D33" s="13"/>
-      <c r="E33" s="45" t="s">
-        <v>179</v>
+      <c r="E33" s="46" t="s">
+        <v>175</v>
       </c>
       <c r="F33" s="13"/>
-      <c r="G33" s="46"/>
+      <c r="G33" s="47"/>
       <c r="H33" s="13"/>
-      <c r="I33" s="46"/>
+      <c r="I33" s="47"/>
       <c r="J33" s="13"/>
-      <c r="K33" s="46"/>
+      <c r="K33" s="47"/>
       <c r="L33" s="13"/>
-      <c r="M33" s="42"/>
+      <c r="M33" s="43"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="37">
         <v>0.60416666666666663</v>
       </c>
       <c r="B34" s="34"/>
-      <c r="C34" s="47"/>
+      <c r="C34" s="48"/>
       <c r="D34" s="13"/>
-      <c r="E34" s="47"/>
+      <c r="E34" s="48"/>
       <c r="F34" s="13"/>
-      <c r="G34" s="47"/>
+      <c r="G34" s="48"/>
       <c r="H34" s="13"/>
-      <c r="I34" s="47"/>
+      <c r="I34" s="48"/>
       <c r="J34" s="13"/>
-      <c r="K34" s="47"/>
+      <c r="K34" s="48"/>
       <c r="L34" s="13"/>
-      <c r="M34" s="42"/>
+      <c r="M34" s="43"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="37"/>
       <c r="B35" s="34"/>
       <c r="C35" s="36"/>
@@ -3251,526 +3652,526 @@
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
-      <c r="M35" s="42"/>
+      <c r="M35" s="43"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
     </row>
-    <row r="36" spans="1:15" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="37"/>
       <c r="B36" s="34"/>
-      <c r="C36" s="45" t="s">
-        <v>174</v>
+      <c r="C36" s="46" t="s">
+        <v>170</v>
       </c>
       <c r="D36" s="13"/>
-      <c r="E36" s="45" t="s">
-        <v>180</v>
+      <c r="E36" s="46" t="s">
+        <v>176</v>
       </c>
       <c r="F36" s="13"/>
-      <c r="G36" s="45" t="s">
-        <v>185</v>
+      <c r="G36" s="46" t="s">
+        <v>181</v>
       </c>
       <c r="H36" s="13"/>
-      <c r="I36" s="45" t="s">
+      <c r="I36" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="J36" s="45"/>
+      <c r="K36" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="J36" s="44"/>
-      <c r="K36" s="45" t="s">
-        <v>192</v>
-      </c>
       <c r="L36" s="13"/>
-      <c r="M36" s="43"/>
+      <c r="M36" s="44"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="37"/>
       <c r="B37" s="34"/>
-      <c r="C37" s="46"/>
+      <c r="C37" s="47"/>
       <c r="D37" s="13"/>
-      <c r="E37" s="46"/>
+      <c r="E37" s="47"/>
       <c r="F37" s="13"/>
-      <c r="G37" s="46"/>
+      <c r="G37" s="47"/>
       <c r="H37" s="13"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="46"/>
+      <c r="I37" s="47"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="47"/>
       <c r="L37" s="13"/>
       <c r="M37" s="13"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="1:15" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="37">
         <v>0.625</v>
       </c>
       <c r="B38" s="34"/>
-      <c r="C38" s="47"/>
+      <c r="C38" s="48"/>
       <c r="D38" s="13"/>
-      <c r="E38" s="47"/>
+      <c r="E38" s="48"/>
       <c r="F38" s="13"/>
-      <c r="G38" s="46"/>
+      <c r="G38" s="47"/>
       <c r="H38" s="13"/>
-      <c r="I38" s="46"/>
-      <c r="J38" s="44"/>
-      <c r="K38" s="46"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="47"/>
       <c r="L38" s="13"/>
-      <c r="M38" s="41" t="s">
-        <v>148</v>
+      <c r="M38" s="42" t="s">
+        <v>147</v>
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="37"/>
       <c r="B39" s="34"/>
       <c r="C39" s="33"/>
-      <c r="D39" s="44"/>
+      <c r="D39" s="45"/>
       <c r="E39" s="33"/>
       <c r="F39" s="13"/>
-      <c r="G39" s="46"/>
+      <c r="G39" s="47"/>
       <c r="H39" s="13"/>
-      <c r="I39" s="46"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="46"/>
+      <c r="I39" s="47"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="47"/>
       <c r="L39" s="13"/>
-      <c r="M39" s="42"/>
+      <c r="M39" s="43"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="37"/>
       <c r="B40" s="34"/>
-      <c r="C40" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="D40" s="44"/>
-      <c r="E40" s="45" t="s">
-        <v>181</v>
+      <c r="C40" s="46" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" s="45"/>
+      <c r="E40" s="46" t="s">
+        <v>177</v>
       </c>
       <c r="F40" s="13"/>
-      <c r="G40" s="46"/>
+      <c r="G40" s="47"/>
       <c r="H40" s="13"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="47"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="45"/>
+      <c r="K40" s="48"/>
       <c r="L40" s="13"/>
-      <c r="M40" s="42"/>
+      <c r="M40" s="43"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
     </row>
-    <row r="41" spans="1:15" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="37">
         <v>0.64583333333333337</v>
       </c>
       <c r="B41" s="34"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="46"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="47"/>
       <c r="F41" s="13"/>
-      <c r="G41" s="46"/>
+      <c r="G41" s="47"/>
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
-      <c r="J41" s="44"/>
+      <c r="J41" s="45"/>
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
-      <c r="M41" s="42"/>
+      <c r="M41" s="43"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
     </row>
-    <row r="42" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="37"/>
       <c r="B42" s="34"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="47"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="48"/>
       <c r="F42" s="13"/>
-      <c r="G42" s="46"/>
+      <c r="G42" s="47"/>
       <c r="H42" s="13"/>
-      <c r="I42" s="45" t="s">
+      <c r="I42" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="J42" s="45"/>
+      <c r="K42" s="46" t="s">
         <v>189</v>
       </c>
-      <c r="J42" s="44"/>
-      <c r="K42" s="45" t="s">
-        <v>193</v>
-      </c>
       <c r="L42" s="13"/>
-      <c r="M42" s="42"/>
+      <c r="M42" s="43"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="37"/>
       <c r="B43" s="34"/>
       <c r="C43" s="32"/>
       <c r="D43" s="13"/>
       <c r="E43" s="33"/>
       <c r="F43" s="13"/>
-      <c r="G43" s="47"/>
+      <c r="G43" s="48"/>
       <c r="H43" s="13"/>
-      <c r="I43" s="46"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="46"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="47"/>
       <c r="L43" s="13"/>
-      <c r="M43" s="42"/>
+      <c r="M43" s="43"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
     </row>
-    <row r="44" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="37"/>
       <c r="B44" s="34"/>
-      <c r="C44" s="45" t="s">
-        <v>197</v>
+      <c r="C44" s="46" t="s">
+        <v>193</v>
       </c>
       <c r="D44" s="13"/>
-      <c r="E44" s="45" t="s">
-        <v>182</v>
+      <c r="E44" s="46" t="s">
+        <v>178</v>
       </c>
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="46"/>
+      <c r="I44" s="47"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="47"/>
       <c r="L44" s="13"/>
-      <c r="M44" s="43"/>
+      <c r="M44" s="44"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
     </row>
-    <row r="45" spans="1:15" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="37">
         <v>0.66666666666666663</v>
       </c>
       <c r="B45" s="34"/>
-      <c r="C45" s="46"/>
+      <c r="C45" s="47"/>
       <c r="D45" s="13"/>
-      <c r="E45" s="46"/>
+      <c r="E45" s="47"/>
       <c r="F45" s="13"/>
-      <c r="G45" s="45" t="s">
-        <v>186</v>
+      <c r="G45" s="46" t="s">
+        <v>182</v>
       </c>
       <c r="H45" s="13"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="46"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="45"/>
+      <c r="K45" s="47"/>
       <c r="L45" s="13"/>
       <c r="M45" s="13"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="1:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="37"/>
       <c r="B46" s="34"/>
-      <c r="C46" s="46"/>
+      <c r="C46" s="47"/>
       <c r="D46" s="13"/>
-      <c r="E46" s="46"/>
+      <c r="E46" s="47"/>
       <c r="F46" s="13"/>
-      <c r="G46" s="46"/>
+      <c r="G46" s="47"/>
       <c r="H46" s="13"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="44"/>
-      <c r="K46" s="46"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="45"/>
+      <c r="K46" s="47"/>
       <c r="L46" s="13"/>
-      <c r="M46" s="41" t="s">
-        <v>147</v>
+      <c r="M46" s="42" t="s">
+        <v>146</v>
       </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="37"/>
       <c r="B47" s="34"/>
-      <c r="C47" s="46"/>
+      <c r="C47" s="47"/>
       <c r="D47" s="13"/>
-      <c r="E47" s="46"/>
+      <c r="E47" s="47"/>
       <c r="F47" s="13"/>
-      <c r="G47" s="46"/>
+      <c r="G47" s="47"/>
       <c r="H47" s="13"/>
-      <c r="I47" s="47"/>
-      <c r="J47" s="44"/>
-      <c r="K47" s="47"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="45"/>
+      <c r="K47" s="48"/>
       <c r="L47" s="13"/>
-      <c r="M47" s="42"/>
+      <c r="M47" s="43"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
     </row>
-    <row r="48" spans="1:15" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="37"/>
       <c r="B48" s="34"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="44"/>
-      <c r="E48" s="47"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="48"/>
       <c r="F48" s="13"/>
-      <c r="G48" s="46"/>
+      <c r="G48" s="47"/>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
-      <c r="M48" s="42"/>
+      <c r="M48" s="43"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
     </row>
-    <row r="49" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="37"/>
       <c r="B49" s="34"/>
       <c r="C49" s="32"/>
-      <c r="D49" s="44"/>
+      <c r="D49" s="45"/>
       <c r="E49" s="33"/>
       <c r="F49" s="13"/>
-      <c r="G49" s="46"/>
+      <c r="G49" s="47"/>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
       <c r="K49" s="13"/>
       <c r="L49" s="13"/>
-      <c r="M49" s="42"/>
+      <c r="M49" s="43"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
     </row>
-    <row r="50" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="37">
         <v>0.6875</v>
       </c>
       <c r="B50" s="34"/>
-      <c r="C50" s="45" t="s">
-        <v>176</v>
-      </c>
-      <c r="D50" s="44"/>
-      <c r="E50" s="45" t="s">
-        <v>183</v>
+      <c r="C50" s="46" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" s="45"/>
+      <c r="E50" s="46" t="s">
+        <v>179</v>
       </c>
       <c r="F50" s="13"/>
-      <c r="G50" s="46"/>
+      <c r="G50" s="47"/>
       <c r="H50" s="13"/>
-      <c r="I50" s="45" t="s">
+      <c r="I50" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="J50" s="13"/>
+      <c r="K50" s="46" t="s">
         <v>190</v>
       </c>
-      <c r="J50" s="13"/>
-      <c r="K50" s="45" t="s">
-        <v>194</v>
-      </c>
       <c r="L50" s="13"/>
-      <c r="M50" s="42"/>
+      <c r="M50" s="43"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
     </row>
-    <row r="51" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="37"/>
       <c r="B51" s="34"/>
-      <c r="C51" s="46"/>
+      <c r="C51" s="47"/>
       <c r="D51" s="13"/>
-      <c r="E51" s="46"/>
+      <c r="E51" s="47"/>
       <c r="F51" s="13"/>
-      <c r="G51" s="46"/>
+      <c r="G51" s="47"/>
       <c r="H51" s="13"/>
-      <c r="I51" s="46"/>
+      <c r="I51" s="47"/>
       <c r="J51" s="13"/>
-      <c r="K51" s="46"/>
+      <c r="K51" s="47"/>
       <c r="L51" s="13"/>
-      <c r="M51" s="42"/>
+      <c r="M51" s="43"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
     </row>
-    <row r="52" spans="1:15" ht="10.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="10.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="37"/>
       <c r="B52" s="34"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="46"/>
+      <c r="C52" s="47"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="47"/>
       <c r="F52" s="13"/>
-      <c r="G52" s="46"/>
+      <c r="G52" s="47"/>
       <c r="H52" s="13"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="44"/>
-      <c r="K52" s="46"/>
+      <c r="I52" s="47"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="47"/>
       <c r="L52" s="13"/>
-      <c r="M52" s="42"/>
+      <c r="M52" s="43"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="37"/>
       <c r="B53" s="34"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="44"/>
-      <c r="E53" s="46"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="47"/>
       <c r="F53" s="13"/>
-      <c r="G53" s="46"/>
+      <c r="G53" s="47"/>
       <c r="H53" s="13"/>
-      <c r="I53" s="46"/>
-      <c r="J53" s="44"/>
-      <c r="K53" s="46"/>
+      <c r="I53" s="47"/>
+      <c r="J53" s="45"/>
+      <c r="K53" s="47"/>
       <c r="L53" s="13"/>
-      <c r="M53" s="42"/>
+      <c r="M53" s="43"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
     </row>
-    <row r="54" spans="1:15" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="37">
         <v>0.70833333333333337</v>
       </c>
       <c r="B54" s="34"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="44"/>
-      <c r="E54" s="46"/>
+      <c r="C54" s="47"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="47"/>
       <c r="F54" s="13"/>
-      <c r="G54" s="47"/>
+      <c r="G54" s="48"/>
       <c r="H54" s="13"/>
-      <c r="I54" s="46"/>
-      <c r="J54" s="44"/>
-      <c r="K54" s="46"/>
+      <c r="I54" s="47"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="47"/>
       <c r="L54" s="13"/>
-      <c r="M54" s="43"/>
+      <c r="M54" s="44"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
     </row>
-    <row r="55" spans="1:15" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="37"/>
       <c r="B55" s="34"/>
-      <c r="C55" s="46"/>
-      <c r="D55" s="44"/>
-      <c r="E55" s="46"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="47"/>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
-      <c r="I55" s="46"/>
-      <c r="J55" s="44"/>
-      <c r="K55" s="46"/>
+      <c r="I55" s="47"/>
+      <c r="J55" s="45"/>
+      <c r="K55" s="47"/>
       <c r="L55" s="13"/>
       <c r="M55" s="13"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
     </row>
-    <row r="56" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="37"/>
       <c r="B56" s="34"/>
-      <c r="C56" s="46"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="46"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="47"/>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
-      <c r="I56" s="47"/>
-      <c r="J56" s="44"/>
-      <c r="K56" s="47"/>
+      <c r="I56" s="48"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="48"/>
       <c r="L56" s="13"/>
-      <c r="M56" s="41" t="s">
-        <v>142</v>
+      <c r="M56" s="42" t="s">
+        <v>141</v>
       </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
     </row>
-    <row r="57" spans="1:15" ht="10.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="10.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="37"/>
       <c r="B57" s="34"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="44"/>
-      <c r="E57" s="47"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="48"/>
       <c r="F57" s="13"/>
-      <c r="G57" s="45" t="s">
-        <v>157</v>
+      <c r="G57" s="46" t="s">
+        <v>155</v>
       </c>
       <c r="H57" s="13"/>
       <c r="I57" s="13"/>
-      <c r="J57" s="44"/>
+      <c r="J57" s="45"/>
       <c r="K57" s="13"/>
       <c r="L57" s="13"/>
-      <c r="M57" s="42"/>
+      <c r="M57" s="43"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
     </row>
-    <row r="58" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="37"/>
       <c r="B58" s="34"/>
       <c r="C58" s="33"/>
-      <c r="D58" s="44"/>
+      <c r="D58" s="45"/>
       <c r="E58" s="33"/>
       <c r="F58" s="13"/>
-      <c r="G58" s="46"/>
+      <c r="G58" s="47"/>
       <c r="H58" s="13"/>
-      <c r="I58" s="45" t="s">
-        <v>198</v>
-      </c>
-      <c r="J58" s="44"/>
-      <c r="K58" s="45" t="s">
-        <v>143</v>
+      <c r="I58" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="J58" s="45"/>
+      <c r="K58" s="46" t="s">
+        <v>142</v>
       </c>
       <c r="L58" s="13"/>
-      <c r="M58" s="42"/>
+      <c r="M58" s="43"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
     </row>
-    <row r="59" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="37">
         <v>0.72916666666666663</v>
       </c>
       <c r="B59" s="34"/>
-      <c r="C59" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="D59" s="44"/>
-      <c r="E59" s="45" t="s">
-        <v>146</v>
+      <c r="C59" s="46" t="s">
+        <v>173</v>
+      </c>
+      <c r="D59" s="45"/>
+      <c r="E59" s="46" t="s">
+        <v>145</v>
       </c>
       <c r="F59" s="13"/>
-      <c r="G59" s="46"/>
+      <c r="G59" s="47"/>
       <c r="H59" s="13"/>
-      <c r="I59" s="46"/>
-      <c r="J59" s="44"/>
-      <c r="K59" s="46"/>
+      <c r="I59" s="47"/>
+      <c r="J59" s="45"/>
+      <c r="K59" s="47"/>
       <c r="L59" s="13"/>
-      <c r="M59" s="42"/>
+      <c r="M59" s="43"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
     </row>
-    <row r="60" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="37"/>
       <c r="B60" s="34"/>
-      <c r="C60" s="47"/>
+      <c r="C60" s="48"/>
       <c r="D60" s="13"/>
-      <c r="E60" s="47"/>
+      <c r="E60" s="48"/>
       <c r="F60" s="13"/>
-      <c r="G60" s="46"/>
+      <c r="G60" s="47"/>
       <c r="H60" s="13"/>
-      <c r="I60" s="46"/>
+      <c r="I60" s="47"/>
       <c r="J60" s="13"/>
-      <c r="K60" s="46"/>
+      <c r="K60" s="47"/>
       <c r="L60" s="13"/>
-      <c r="M60" s="42"/>
+      <c r="M60" s="43"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
     </row>
-    <row r="61" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="37"/>
       <c r="B61" s="34"/>
       <c r="C61" s="33"/>
       <c r="D61" s="13"/>
       <c r="E61" s="33"/>
       <c r="F61" s="13"/>
-      <c r="G61" s="46"/>
+      <c r="G61" s="47"/>
       <c r="H61" s="13"/>
-      <c r="I61" s="47"/>
+      <c r="I61" s="48"/>
       <c r="J61" s="13"/>
-      <c r="K61" s="47"/>
+      <c r="K61" s="48"/>
       <c r="L61" s="13"/>
-      <c r="M61" s="43"/>
+      <c r="M61" s="44"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
     </row>
-    <row r="62" spans="1:15" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="37">
         <v>0.75</v>
       </c>
       <c r="B62" s="34"/>
-      <c r="C62" s="45" t="s">
-        <v>196</v>
+      <c r="C62" s="46" t="s">
+        <v>192</v>
       </c>
       <c r="D62" s="13"/>
-      <c r="E62" s="45" t="s">
-        <v>195</v>
+      <c r="E62" s="46" t="s">
+        <v>191</v>
       </c>
       <c r="F62" s="13"/>
-      <c r="G62" s="47"/>
+      <c r="G62" s="48"/>
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
       <c r="J62" s="13"/>
@@ -3780,130 +4181,130 @@
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
     </row>
-    <row r="63" spans="1:15" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="37"/>
       <c r="B63" s="34"/>
-      <c r="C63" s="47"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="47"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="48"/>
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
-      <c r="J63" s="44"/>
+      <c r="J63" s="45"/>
       <c r="K63" s="13"/>
       <c r="L63" s="13"/>
       <c r="M63" s="13"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
     </row>
-    <row r="64" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="37"/>
       <c r="B64" s="34"/>
       <c r="C64" s="33"/>
-      <c r="D64" s="44"/>
+      <c r="D64" s="45"/>
       <c r="E64" s="33"/>
       <c r="F64" s="13"/>
       <c r="G64" s="13"/>
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
-      <c r="J64" s="44"/>
+      <c r="J64" s="45"/>
       <c r="K64" s="13"/>
       <c r="L64" s="13"/>
       <c r="M64" s="13"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
     </row>
-    <row r="65" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="37">
         <v>0.77083333333333337</v>
       </c>
       <c r="B65" s="34"/>
       <c r="C65" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="D65" s="44"/>
+        <v>140</v>
+      </c>
+      <c r="D65" s="45"/>
       <c r="E65" s="33"/>
       <c r="F65" s="13"/>
       <c r="G65" s="13"/>
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
-      <c r="J65" s="44"/>
+      <c r="J65" s="45"/>
       <c r="K65" s="13"/>
       <c r="L65" s="13"/>
       <c r="M65" s="13"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
     </row>
-    <row r="66" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="37"/>
       <c r="B66" s="34"/>
       <c r="C66" s="33"/>
-      <c r="D66" s="44"/>
+      <c r="D66" s="45"/>
       <c r="E66" s="33"/>
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
-      <c r="J66" s="44"/>
+      <c r="J66" s="45"/>
       <c r="K66" s="13"/>
       <c r="L66" s="13"/>
       <c r="M66" s="13"/>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
     </row>
-    <row r="67" spans="1:15" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="37"/>
       <c r="B67" s="34"/>
       <c r="C67" s="33"/>
-      <c r="D67" s="44"/>
+      <c r="D67" s="45"/>
       <c r="E67" s="33"/>
       <c r="F67" s="13"/>
       <c r="G67" s="13"/>
       <c r="H67" s="13"/>
       <c r="I67" s="13"/>
-      <c r="J67" s="44"/>
+      <c r="J67" s="45"/>
       <c r="K67" s="13"/>
       <c r="L67" s="13"/>
       <c r="M67" s="13"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
     </row>
-    <row r="68" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="30"/>
       <c r="B68" s="34"/>
       <c r="C68" s="33"/>
-      <c r="D68" s="44"/>
+      <c r="D68" s="45"/>
       <c r="E68" s="33"/>
       <c r="F68" s="13"/>
       <c r="G68" s="13"/>
       <c r="H68" s="13"/>
       <c r="I68" s="13"/>
-      <c r="J68" s="44"/>
+      <c r="J68" s="45"/>
       <c r="K68" s="13"/>
       <c r="L68" s="13"/>
       <c r="M68" s="13"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
     </row>
-    <row r="69" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="30"/>
       <c r="B69" s="34"/>
       <c r="C69" s="33"/>
-      <c r="D69" s="44"/>
+      <c r="D69" s="45"/>
       <c r="E69" s="33"/>
       <c r="F69" s="13"/>
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
-      <c r="J69" s="44"/>
+      <c r="J69" s="45"/>
       <c r="K69" s="13"/>
       <c r="L69" s="13"/>
       <c r="M69" s="13"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
     </row>
-    <row r="70" spans="1:15" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="24"/>
       <c r="B70" s="1"/>
       <c r="C70" s="20"/>
@@ -3920,7 +4321,7 @@
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
     </row>
-    <row r="71" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="24"/>
       <c r="B71" s="1"/>
       <c r="C71" s="18"/>
@@ -3937,7 +4338,7 @@
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
     </row>
-    <row r="72" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="24"/>
       <c r="B72" s="1"/>
       <c r="C72" s="18"/>
@@ -3954,109 +4355,109 @@
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
     </row>
-    <row r="73" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="24"/>
       <c r="B73" s="1"/>
       <c r="C73" s="23"/>
-      <c r="D73" s="44"/>
+      <c r="D73" s="45"/>
       <c r="E73" s="23"/>
       <c r="F73" s="1"/>
       <c r="G73" s="6"/>
       <c r="H73" s="1"/>
       <c r="I73" s="6"/>
-      <c r="J73" s="44"/>
+      <c r="J73" s="45"/>
       <c r="K73" s="6"/>
       <c r="L73" s="1"/>
       <c r="M73" s="6"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
     </row>
-    <row r="74" spans="1:15" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="24"/>
       <c r="B74" s="1"/>
       <c r="C74" s="23"/>
-      <c r="D74" s="44"/>
+      <c r="D74" s="45"/>
       <c r="E74" s="23"/>
       <c r="F74" s="1"/>
       <c r="G74" s="6"/>
       <c r="H74" s="1"/>
       <c r="I74" s="6"/>
-      <c r="J74" s="44"/>
+      <c r="J74" s="45"/>
       <c r="K74" s="6"/>
       <c r="L74" s="1"/>
       <c r="M74" s="6"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
     </row>
-    <row r="75" spans="1:15" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="24"/>
       <c r="B75" s="1"/>
       <c r="C75" s="23"/>
-      <c r="D75" s="44"/>
+      <c r="D75" s="45"/>
       <c r="E75" s="23"/>
       <c r="F75" s="1"/>
       <c r="G75" s="6"/>
       <c r="H75" s="1"/>
       <c r="I75" s="6"/>
-      <c r="J75" s="44"/>
+      <c r="J75" s="45"/>
       <c r="K75" s="6"/>
       <c r="L75" s="1"/>
       <c r="M75" s="6"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
     </row>
-    <row r="76" spans="1:15" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="24"/>
       <c r="B76" s="1"/>
       <c r="C76" s="23"/>
-      <c r="D76" s="44"/>
+      <c r="D76" s="45"/>
       <c r="E76" s="23"/>
       <c r="F76" s="1"/>
       <c r="G76" s="6"/>
       <c r="H76" s="1"/>
       <c r="I76" s="6"/>
-      <c r="J76" s="44"/>
+      <c r="J76" s="45"/>
       <c r="K76" s="6"/>
       <c r="L76" s="1"/>
       <c r="M76" s="6"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="24"/>
       <c r="B77" s="1"/>
       <c r="C77" s="23"/>
-      <c r="D77" s="44"/>
+      <c r="D77" s="45"/>
       <c r="E77" s="23"/>
       <c r="F77" s="1"/>
       <c r="G77" s="6"/>
       <c r="H77" s="1"/>
       <c r="I77" s="6"/>
-      <c r="J77" s="44"/>
+      <c r="J77" s="45"/>
       <c r="K77" s="6"/>
       <c r="L77" s="1"/>
       <c r="M77" s="6"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
     </row>
-    <row r="78" spans="1:15" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="24"/>
       <c r="B78" s="1"/>
       <c r="C78" s="23"/>
-      <c r="D78" s="44"/>
+      <c r="D78" s="45"/>
       <c r="E78" s="23"/>
       <c r="F78" s="1"/>
       <c r="G78" s="6"/>
       <c r="H78" s="1"/>
       <c r="I78" s="6"/>
-      <c r="J78" s="44"/>
+      <c r="J78" s="45"/>
       <c r="K78" s="6"/>
       <c r="L78" s="1"/>
       <c r="M78" s="6"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
     </row>
-    <row r="79" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="24"/>
       <c r="B79" s="1"/>
       <c r="C79" s="18"/>
@@ -4066,14 +4467,14 @@
       <c r="G79" s="6"/>
       <c r="H79" s="1"/>
       <c r="I79" s="6"/>
-      <c r="J79" s="44"/>
+      <c r="J79" s="45"/>
       <c r="K79" s="6"/>
       <c r="L79" s="1"/>
       <c r="M79" s="6"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
     </row>
-    <row r="80" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="24"/>
       <c r="B80" s="1"/>
       <c r="C80" s="18"/>
@@ -4083,69 +4484,69 @@
       <c r="G80" s="6"/>
       <c r="H80" s="1"/>
       <c r="I80" s="6"/>
-      <c r="J80" s="44"/>
+      <c r="J80" s="45"/>
       <c r="K80" s="6"/>
       <c r="L80" s="1"/>
       <c r="M80" s="6"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
     </row>
-    <row r="81" spans="1:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="24"/>
       <c r="B81" s="1"/>
       <c r="C81" s="23"/>
-      <c r="D81" s="44"/>
+      <c r="D81" s="45"/>
       <c r="E81" s="23"/>
       <c r="F81" s="1"/>
       <c r="G81" s="6"/>
       <c r="H81" s="1"/>
       <c r="I81" s="6"/>
-      <c r="J81" s="44"/>
+      <c r="J81" s="45"/>
       <c r="K81" s="6"/>
       <c r="L81" s="1"/>
       <c r="M81" s="6"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
     </row>
-    <row r="82" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="24"/>
       <c r="B82" s="1"/>
       <c r="C82" s="23"/>
-      <c r="D82" s="44"/>
+      <c r="D82" s="45"/>
       <c r="E82" s="23"/>
       <c r="F82" s="1"/>
       <c r="G82" s="6"/>
       <c r="H82" s="1"/>
       <c r="I82" s="6"/>
-      <c r="J82" s="44"/>
+      <c r="J82" s="45"/>
       <c r="K82" s="6"/>
       <c r="L82" s="1"/>
       <c r="M82" s="6"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
     </row>
-    <row r="83" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="24"/>
       <c r="B83" s="1"/>
       <c r="C83" s="23"/>
-      <c r="D83" s="44"/>
+      <c r="D83" s="45"/>
       <c r="E83" s="23"/>
       <c r="F83" s="1"/>
       <c r="G83" s="6"/>
       <c r="H83" s="1"/>
       <c r="I83" s="6"/>
-      <c r="J83" s="44"/>
+      <c r="J83" s="45"/>
       <c r="K83" s="6"/>
       <c r="L83" s="1"/>
       <c r="M83" s="6"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" s="24"/>
       <c r="B84" s="1"/>
       <c r="C84" s="23"/>
-      <c r="D84" s="44"/>
+      <c r="D84" s="45"/>
       <c r="E84" s="23"/>
       <c r="F84" s="1"/>
       <c r="G84" s="6"/>
@@ -4158,7 +4559,7 @@
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
     </row>
-    <row r="85" spans="1:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="24"/>
       <c r="B85" s="1"/>
       <c r="C85" s="7"/>
@@ -4175,53 +4576,53 @@
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
     </row>
-    <row r="86" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="27"/>
     </row>
-    <row r="87" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="27"/>
     </row>
-    <row r="88" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="27"/>
     </row>
-    <row r="89" spans="1:15" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="27"/>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="27"/>
     </row>
-    <row r="91" spans="1:15" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="27"/>
     </row>
-    <row r="92" spans="1:15" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="27"/>
     </row>
-    <row r="93" spans="1:15" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="27"/>
     </row>
-    <row r="94" spans="1:15" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="27"/>
     </row>
-    <row r="95" spans="1:15" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="27"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" s="27"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="27"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="27"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="27"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="54"/>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="54"/>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="55"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="76">
@@ -4243,10 +4644,10 @@
     <mergeCell ref="K36:K40"/>
     <mergeCell ref="K16:K19"/>
     <mergeCell ref="K21:K25"/>
-    <mergeCell ref="M13:M17"/>
     <mergeCell ref="M19:M22"/>
-    <mergeCell ref="M7:M11"/>
     <mergeCell ref="M24:M29"/>
+    <mergeCell ref="M14:M18"/>
+    <mergeCell ref="M10:M13"/>
     <mergeCell ref="C36:C38"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="E10:E13"/>
@@ -4356,6 +4757,9 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
+  <customProperties>
+    <customPr name="_pios_id" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -4366,23 +4770,23 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" customWidth="1"/>
-    <col min="7" max="7" width="88.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="41.5546875" customWidth="1"/>
+    <col min="7" max="7" width="88.109375" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>8</v>
@@ -4406,7 +4810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>0.41666666666666669</v>
       </c>
@@ -4417,22 +4821,22 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
       <c r="B3" s="11">
         <v>0.44444444444444442</v>
       </c>
@@ -4440,22 +4844,22 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B4" s="11">
         <v>0.44444444444444442</v>
       </c>
@@ -4463,22 +4867,22 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="B5" s="11">
         <v>0.4513888888888889</v>
       </c>
@@ -4492,16 +4896,16 @@
         <v>21</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="11">
         <v>0.4513888888888889</v>
       </c>
@@ -4512,17 +4916,17 @@
         <v>12</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>0.45833333333333331</v>
       </c>
@@ -4533,22 +4937,22 @@
         <v>0.50694444444444442</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B8" s="11">
         <v>0.47916666666666669</v>
       </c>
@@ -4556,22 +4960,22 @@
         <v>0.50694444444444442</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B9" s="11">
         <v>0.4861111111111111</v>
       </c>
@@ -4585,16 +4989,16 @@
         <v>32</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="11">
         <v>0.4861111111111111</v>
       </c>
@@ -4605,17 +5009,17 @@
         <v>12</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>0.5</v>
       </c>
@@ -4626,22 +5030,22 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="11">
         <v>0.51388888888888895</v>
       </c>
@@ -4649,22 +5053,22 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="11">
         <v>0.52083333333333337</v>
       </c>
@@ -4678,16 +5082,16 @@
         <v>24</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
         <v>0.52083333333333337</v>
       </c>
@@ -4701,16 +5105,16 @@
         <v>27</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="29">
         <v>0.54166666666666663</v>
       </c>
@@ -4721,22 +5125,22 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B16" s="11">
         <v>0.5625</v>
       </c>
@@ -4744,20 +5148,20 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B17" s="11">
         <v>0.56944444444444442</v>
       </c>
@@ -4765,22 +5169,22 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18" s="11">
         <v>0.58333333333333337</v>
       </c>
@@ -4794,16 +5198,16 @@
         <v>30</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="29">
         <v>0.58333333333333337</v>
       </c>
@@ -4817,17 +5221,17 @@
         <v>12</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B20" s="11">
         <v>0.59722222222222221</v>
       </c>
@@ -4835,20 +5239,20 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B21" s="11">
         <v>0.59722222222222221</v>
       </c>
@@ -4856,20 +5260,20 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B22" s="11">
         <v>0.61805555555555558</v>
       </c>
@@ -4877,22 +5281,22 @@
         <v>0.65972222222222221</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B23" s="11">
         <v>0.61805555555555558</v>
       </c>
@@ -4903,19 +5307,19 @@
         <v>11</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B24" s="11">
         <v>0.61805555555555558</v>
       </c>
@@ -4923,22 +5327,22 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>0.625</v>
       </c>
@@ -4949,20 +5353,20 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H25" s="12"/>
     </row>
-    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B26" s="11">
         <v>0.63888888888888895</v>
       </c>
@@ -4970,20 +5374,20 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>33</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H26" s="12"/>
     </row>
-    <row r="27" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B27" s="11">
         <v>0.65277777777777779</v>
       </c>
@@ -4994,19 +5398,19 @@
         <v>12</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B28" s="11">
         <v>0.65277777777777779</v>
       </c>
@@ -5017,19 +5421,19 @@
         <v>11</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B29" s="11">
         <v>0.65972222222222221</v>
       </c>
@@ -5037,22 +5441,22 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>20</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="B30" s="11">
         <v>0.65972222222222221</v>
       </c>
@@ -5060,22 +5464,22 @@
         <v>0.6875</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B31" s="11">
         <v>0.65972222222222221</v>
       </c>
@@ -5083,22 +5487,22 @@
         <v>0.6875</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <v>0.66666666666666663</v>
       </c>
@@ -5109,22 +5513,22 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B33" s="11">
         <v>0.6875</v>
       </c>
@@ -5135,19 +5539,19 @@
         <v>11</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B34" s="11">
         <v>0.6875</v>
       </c>
@@ -5158,19 +5562,19 @@
         <v>12</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B35" s="11">
         <v>0.69444444444444453</v>
       </c>
@@ -5178,22 +5582,22 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B36" s="11">
         <v>0.70138888888888884</v>
       </c>
@@ -5201,22 +5605,22 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H36" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="11">
         <v>0.70833333333333337</v>
       </c>
@@ -5227,22 +5631,22 @@
         <v>0.75694444444444453</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>28</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B38" s="11">
         <v>0.72222222222222221</v>
       </c>
@@ -5253,17 +5657,17 @@
         <v>11</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G38" s="9"/>
       <c r="H38" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="B39" s="11">
         <v>0.72916666666666663</v>
       </c>
@@ -5271,22 +5675,22 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B40" s="11">
         <v>0.72916666666666663</v>
       </c>
@@ -5294,22 +5698,22 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
         <v>0.75</v>
       </c>
@@ -5320,22 +5724,22 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="B42" s="11">
         <v>0.75</v>
       </c>
@@ -5343,25 +5747,25 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G43" s="9"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G44" s="9"/>
     </row>
   </sheetData>
@@ -5370,5 +5774,8 @@
   </sortState>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="48" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <customProperties>
+    <customPr name="_pios_id" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UI5con: extend speaker list
</commit_message>
<xml_diff>
--- a/ui5con/downloads/ui5con_2017_agenda.xlsx
+++ b/ui5con/downloads/ui5con_2017_agenda.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D038767\Documents\UI5con\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D050079\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1392" yWindow="0" windowWidth="23040" windowHeight="7920"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="23040" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda UI5con@SAP" sheetId="1" r:id="rId1"/>
@@ -133,6 +133,9 @@
     <t>Aparna Narayanaswamy</t>
   </si>
   <si>
+    <t>Michael Graf</t>
+  </si>
+  <si>
     <t>HP Seitz</t>
   </si>
   <si>
@@ -819,6 +822,29 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>EMBEDDED ANALYTICS WITH CHARTS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Pia Kinkel, Christoph Laux, Bohdan Pukalskyi 
+11:00 - 12:00</t>
+    </r>
+  </si>
+  <si>
     <t>Advanced Charting Controls Coming to UI5</t>
   </si>
   <si>
@@ -1084,6 +1110,29 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t>UI5 CONTROLS FOR DOCUMENT HANDLING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Pia Kinkel, Christoph Laux
+10:00 - 11:00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t>DEVELOPING CUSTOM ESLINT RULES</t>
     </r>
     <r>
@@ -1199,6 +1248,29 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
+      <t>COLLABORATORS WANTED FOR UI5LAB - A CUSTOM UI5 REPO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Michael Graf, Emmanuele Ricci
+14:20 - 14:40                                          </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">MIXED REALITY WITH OPENUI5
 </t>
     </r>
@@ -1810,88 +1882,13 @@
       </rPr>
       <t>AGENDA 2017</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>COLLABORATORS WANTED FOR UI5LAB - A CUSTOM UI5 REPO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Michael Graf, Emanuele Ricci
-14:20 - 14:40                                          </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>UI5 CONTROLS FOR DOCUMENT HANDLING</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Pia Kinkel, Christoph Laux
-10:40 - 11:20</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>EMBEDDED ANALYTICS WITH CHARTS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="0"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Pia Kinkel, Christoph Laux, Bohdan Pukalskyi 
-11:20 - 12:00</t>
-    </r>
-  </si>
-  <si>
-    <t>Michael Graf, Emanuele Ricci</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="###,000"/>
-  </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1991,91 +1988,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF1F497D"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF1F497D"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF00CC00"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF33CC33"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFF9900"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="8"/>
-      <color rgb="FF1F497D"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="8"/>
-      <color rgb="FF1F497D"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="20">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2088,110 +2002,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDBE5F1"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF1F5FB"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE9EFF7"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6F9C1"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFABEDA5"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF94D88F"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFDBF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFB8C"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF843"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF988C"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF6758"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDBE5F1"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB7CFE8"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC3D6EB"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDBE5F2"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2251,187 +2063,10 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="3" tint="-0.24994659260841701"/>
-      </left>
-      <right style="thin">
-        <color theme="3" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="3" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3" tint="0.59996337778862885"/>
-      </left>
-      <right style="thin">
-        <color theme="3" tint="0.59996337778862885"/>
-      </right>
-      <top style="thin">
-        <color theme="3" tint="0.59996337778862885"/>
-      </top>
-      <bottom style="thin">
-        <color theme="3" tint="0.59996337778862885"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FFC0C0C0"/>
-      </left>
-      <right style="hair">
-        <color rgb="FFC0C0C0"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="38">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="8" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="12" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="14" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="15" borderId="8" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="5" borderId="7" applyNumberFormat="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="6" borderId="6" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="6" borderId="7" applyNumberFormat="0" applyBorder="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2549,7 +2184,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2592,46 +2226,11 @@
     <xf numFmtId="20" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="38">
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="SAPBorder" xfId="20"/>
-    <cellStyle name="SAPDataCell" xfId="3"/>
-    <cellStyle name="SAPDataTotalCell" xfId="4"/>
-    <cellStyle name="SAPDimensionCell" xfId="2"/>
-    <cellStyle name="SAPEditableDataCell" xfId="5"/>
-    <cellStyle name="SAPEditableDataTotalCell" xfId="8"/>
-    <cellStyle name="SAPEmphasized" xfId="28"/>
-    <cellStyle name="SAPEmphasizedEditableDataCell" xfId="30"/>
-    <cellStyle name="SAPEmphasizedEditableDataTotalCell" xfId="31"/>
-    <cellStyle name="SAPEmphasizedLockedDataCell" xfId="34"/>
-    <cellStyle name="SAPEmphasizedLockedDataTotalCell" xfId="35"/>
-    <cellStyle name="SAPEmphasizedReadonlyDataCell" xfId="32"/>
-    <cellStyle name="SAPEmphasizedReadonlyDataTotalCell" xfId="33"/>
-    <cellStyle name="SAPEmphasizedTotal" xfId="29"/>
-    <cellStyle name="SAPExceptionLevel1" xfId="11"/>
-    <cellStyle name="SAPExceptionLevel2" xfId="12"/>
-    <cellStyle name="SAPExceptionLevel3" xfId="13"/>
-    <cellStyle name="SAPExceptionLevel4" xfId="14"/>
-    <cellStyle name="SAPExceptionLevel5" xfId="15"/>
-    <cellStyle name="SAPExceptionLevel6" xfId="16"/>
-    <cellStyle name="SAPExceptionLevel7" xfId="17"/>
-    <cellStyle name="SAPExceptionLevel8" xfId="18"/>
-    <cellStyle name="SAPExceptionLevel9" xfId="19"/>
-    <cellStyle name="SAPFormula" xfId="37"/>
-    <cellStyle name="SAPHierarchyCell0" xfId="23"/>
-    <cellStyle name="SAPHierarchyCell1" xfId="24"/>
-    <cellStyle name="SAPHierarchyCell2" xfId="25"/>
-    <cellStyle name="SAPHierarchyCell3" xfId="26"/>
-    <cellStyle name="SAPHierarchyCell4" xfId="27"/>
-    <cellStyle name="SAPLockedDataCell" xfId="7"/>
-    <cellStyle name="SAPLockedDataTotalCell" xfId="10"/>
-    <cellStyle name="SAPMemberCell" xfId="21"/>
-    <cellStyle name="SAPMemberTotalCell" xfId="22"/>
-    <cellStyle name="SAPMessageText" xfId="36"/>
-    <cellStyle name="SAPReadonlyDataCell" xfId="6"/>
-    <cellStyle name="SAPReadonlyDataTotalCell" xfId="9"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2955,34 +2554,34 @@
   <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4"/>
-    <col min="2" max="2" width="1.44140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="2.109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="2.109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="35.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="2.109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="35.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="2.109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="35.6640625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="2.109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="35.6640625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="2.109375" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="8.85546875" style="4"/>
+    <col min="2" max="2" width="1.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="2.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="2.140625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="35.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="2.140625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="35.7109375" style="4" customWidth="1"/>
+    <col min="14" max="14" width="2.140625" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="24" x14ac:dyDescent="0.4">
-      <c r="C1" s="41" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="3" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.3">
+      <c r="C1" s="55" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="3" customFormat="1" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
@@ -3013,47 +2612,47 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>0.39583333333333331</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="51" t="s">
-        <v>135</v>
+      <c r="C3" s="50" t="s">
+        <v>136</v>
       </c>
       <c r="D3" s="22"/>
-      <c r="E3" s="51" t="s">
-        <v>136</v>
+      <c r="E3" s="50" t="s">
+        <v>137</v>
       </c>
       <c r="F3" s="22"/>
-      <c r="G3" s="49"/>
+      <c r="G3" s="48"/>
       <c r="H3" s="17"/>
-      <c r="I3" s="53"/>
+      <c r="I3" s="52"/>
       <c r="J3" s="22"/>
-      <c r="K3" s="53"/>
+      <c r="K3" s="52"/>
       <c r="L3" s="22"/>
-      <c r="M3" s="49"/>
+      <c r="M3" s="48"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="5"/>
-      <c r="C4" s="52"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="17"/>
-      <c r="E4" s="52"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="17"/>
-      <c r="G4" s="50"/>
+      <c r="G4" s="49"/>
       <c r="H4" s="17"/>
-      <c r="I4" s="54"/>
+      <c r="I4" s="53"/>
       <c r="J4" s="17"/>
-      <c r="K4" s="54"/>
+      <c r="K4" s="53"/>
       <c r="L4" s="17"/>
-      <c r="M4" s="50"/>
+      <c r="M4" s="49"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21"/>
       <c r="B5" s="5"/>
       <c r="C5" s="16"/>
@@ -3070,64 +2669,66 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="37">
         <v>0.41666666666666669</v>
       </c>
       <c r="B6" s="31"/>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="41" t="s">
         <v>138</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="42" t="s">
-        <v>137</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
-      <c r="I6" s="45"/>
+      <c r="I6" s="44"/>
       <c r="J6" s="13"/>
-      <c r="K6" s="45"/>
+      <c r="K6" s="44"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="31"/>
-      <c r="C7" s="43"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="43"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="45"/>
+      <c r="I7" s="44"/>
       <c r="J7" s="13"/>
-      <c r="K7" s="45"/>
+      <c r="K7" s="44"/>
       <c r="L7" s="13"/>
-      <c r="M7" s="6"/>
+      <c r="M7" s="41" t="s">
+        <v>167</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="31"/>
-      <c r="C8" s="44"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="44"/>
+      <c r="E8" s="43"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
-      <c r="I8" s="45"/>
+      <c r="I8" s="44"/>
       <c r="J8" s="13"/>
-      <c r="K8" s="45"/>
+      <c r="K8" s="44"/>
       <c r="L8" s="13"/>
-      <c r="M8" s="6"/>
+      <c r="M8" s="42"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37">
         <v>0.4375</v>
       </c>
@@ -3142,93 +2743,93 @@
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
-      <c r="M9" s="6"/>
+      <c r="M9" s="42"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37"/>
       <c r="B10" s="31"/>
-      <c r="C10" s="46" t="s">
-        <v>156</v>
+      <c r="C10" s="45" t="s">
+        <v>158</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="46" t="s">
-        <v>157</v>
+      <c r="E10" s="45" t="s">
+        <v>159</v>
       </c>
       <c r="F10" s="13"/>
-      <c r="G10" s="46" t="s">
-        <v>158</v>
+      <c r="G10" s="45" t="s">
+        <v>160</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="45"/>
+      <c r="J10" s="44"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="42" t="s">
-        <v>197</v>
-      </c>
+      <c r="M10" s="42"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>0.45833333333333331</v>
       </c>
       <c r="B11" s="31"/>
-      <c r="C11" s="47"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="47"/>
+      <c r="E11" s="46"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="47"/>
+      <c r="G11" s="46"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="J11" s="45"/>
-      <c r="K11" s="46" t="s">
-        <v>160</v>
+      <c r="I11" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="J11" s="44"/>
+      <c r="K11" s="45" t="s">
+        <v>162</v>
       </c>
       <c r="L11" s="13"/>
       <c r="M11" s="43"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" s="26" customFormat="1" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" s="26" customFormat="1" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="39"/>
       <c r="B12" s="31"/>
-      <c r="C12" s="47"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="47"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="47"/>
+      <c r="G12" s="46"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="47"/>
+      <c r="I12" s="46"/>
       <c r="J12" s="13"/>
-      <c r="K12" s="47"/>
+      <c r="K12" s="46"/>
       <c r="L12" s="13"/>
-      <c r="M12" s="43"/>
+      <c r="M12" s="13"/>
       <c r="N12" s="25"/>
       <c r="O12" s="25"/>
     </row>
-    <row r="13" spans="1:15" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="31"/>
-      <c r="C13" s="48"/>
+      <c r="C13" s="47"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="48"/>
+      <c r="E13" s="47"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="48"/>
+      <c r="G13" s="47"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="47"/>
+      <c r="I13" s="46"/>
       <c r="J13" s="13"/>
-      <c r="K13" s="47"/>
+      <c r="K13" s="46"/>
       <c r="L13" s="13"/>
-      <c r="M13" s="44"/>
+      <c r="M13" s="41" t="s">
+        <v>151</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37"/>
       <c r="B14" s="31"/>
       <c r="C14" s="13"/>
@@ -3237,27 +2838,25 @@
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="48"/>
+      <c r="I14" s="47"/>
       <c r="J14" s="13"/>
-      <c r="K14" s="48"/>
+      <c r="K14" s="47"/>
       <c r="L14" s="13"/>
-      <c r="M14" s="42" t="s">
-        <v>198</v>
-      </c>
+      <c r="M14" s="42"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37">
         <v>0.47916666666666669</v>
       </c>
       <c r="B15" s="31"/>
-      <c r="C15" s="46" t="s">
-        <v>167</v>
+      <c r="C15" s="45" t="s">
+        <v>170</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="E15" s="46" t="s">
-        <v>166</v>
+      <c r="E15" s="45" t="s">
+        <v>169</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
@@ -3266,167 +2865,167 @@
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="43"/>
+      <c r="M15" s="42"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37"/>
       <c r="B16" s="31"/>
-      <c r="C16" s="47"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="47"/>
+      <c r="E16" s="46"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
-      <c r="I16" s="46" t="s">
-        <v>161</v>
+      <c r="I16" s="45" t="s">
+        <v>163</v>
       </c>
       <c r="J16" s="13"/>
-      <c r="K16" s="46" t="s">
-        <v>164</v>
+      <c r="K16" s="45" t="s">
+        <v>166</v>
       </c>
       <c r="L16" s="13"/>
-      <c r="M16" s="43"/>
+      <c r="M16" s="42"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="31"/>
-      <c r="C17" s="47"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="13"/>
-      <c r="E17" s="47"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="46" t="s">
-        <v>143</v>
+      <c r="G17" s="45" t="s">
+        <v>144</v>
       </c>
       <c r="H17" s="13"/>
-      <c r="I17" s="47"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="13"/>
-      <c r="K17" s="47"/>
+      <c r="K17" s="46"/>
       <c r="L17" s="13"/>
       <c r="M17" s="43"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="37">
         <v>0.5</v>
       </c>
       <c r="B18" s="31"/>
-      <c r="C18" s="48"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="13"/>
-      <c r="E18" s="48"/>
+      <c r="E18" s="47"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="47"/>
+      <c r="G18" s="46"/>
       <c r="H18" s="13"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="47"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="46"/>
       <c r="L18" s="13"/>
-      <c r="M18" s="44"/>
+      <c r="M18" s="13"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37"/>
       <c r="B19" s="31"/>
       <c r="C19" s="32"/>
       <c r="D19" s="13"/>
       <c r="E19" s="32"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="47"/>
+      <c r="G19" s="46"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="48"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="47"/>
       <c r="L19" s="13"/>
-      <c r="M19" s="42" t="s">
-        <v>144</v>
+      <c r="M19" s="41" t="s">
+        <v>145</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37"/>
       <c r="B20" s="31"/>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="46" t="s">
-        <v>165</v>
-      </c>
       <c r="F20" s="13"/>
-      <c r="G20" s="47"/>
+      <c r="G20" s="46"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
-      <c r="M20" s="43"/>
+      <c r="M20" s="42"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37">
         <v>0.52083333333333337</v>
       </c>
       <c r="B21" s="31"/>
-      <c r="C21" s="47"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="47"/>
+      <c r="E21" s="46"/>
       <c r="F21" s="13"/>
-      <c r="G21" s="47"/>
+      <c r="G21" s="46"/>
       <c r="H21" s="13"/>
-      <c r="I21" s="46" t="s">
-        <v>162</v>
-      </c>
-      <c r="J21" s="45"/>
-      <c r="K21" s="46" t="s">
-        <v>163</v>
+      <c r="I21" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="J21" s="44"/>
+      <c r="K21" s="45" t="s">
+        <v>165</v>
       </c>
       <c r="L21" s="13"/>
-      <c r="M21" s="43"/>
+      <c r="M21" s="42"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="1:15" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37"/>
       <c r="B22" s="31"/>
-      <c r="C22" s="47"/>
+      <c r="C22" s="46"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="47"/>
+      <c r="E22" s="46"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="48"/>
+      <c r="G22" s="47"/>
       <c r="H22" s="13"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="47"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="46"/>
       <c r="L22" s="13"/>
-      <c r="M22" s="44"/>
+      <c r="M22" s="43"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37"/>
       <c r="B23" s="31"/>
-      <c r="C23" s="48"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="48"/>
+      <c r="E23" s="47"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
-      <c r="I23" s="47"/>
+      <c r="I23" s="46"/>
       <c r="J23" s="13"/>
-      <c r="K23" s="47"/>
+      <c r="K23" s="46"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="37">
         <v>0.54166666666666663</v>
       </c>
@@ -3437,17 +3036,17 @@
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
-      <c r="I24" s="47"/>
+      <c r="I24" s="46"/>
       <c r="J24" s="13"/>
-      <c r="K24" s="47"/>
+      <c r="K24" s="46"/>
       <c r="L24" s="13"/>
-      <c r="M24" s="42" t="s">
-        <v>149</v>
+      <c r="M24" s="41" t="s">
+        <v>150</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="1:15" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="31"/>
       <c r="C25" s="13"/>
@@ -3456,15 +3055,15 @@
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
-      <c r="I25" s="48"/>
+      <c r="I25" s="47"/>
       <c r="J25" s="13"/>
-      <c r="K25" s="48"/>
+      <c r="K25" s="47"/>
       <c r="L25" s="13"/>
-      <c r="M25" s="43"/>
+      <c r="M25" s="42"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37"/>
       <c r="B26" s="31"/>
       <c r="C26" s="13"/>
@@ -3477,19 +3076,19 @@
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
-      <c r="M26" s="43"/>
+      <c r="M26" s="42"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37">
         <v>0.5625</v>
       </c>
       <c r="B27" s="31"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
-      <c r="E27" s="46" t="s">
-        <v>174</v>
+      <c r="E27" s="45" t="s">
+        <v>178</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
@@ -3498,56 +3097,56 @@
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
-      <c r="M27" s="43"/>
+      <c r="M27" s="42"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" s="31"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
-      <c r="E28" s="47"/>
+      <c r="E28" s="46"/>
       <c r="F28" s="13"/>
-      <c r="G28" s="46" t="s">
-        <v>180</v>
+      <c r="G28" s="45" t="s">
+        <v>184</v>
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
-      <c r="M28" s="43"/>
+      <c r="M28" s="42"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="31"/>
-      <c r="C29" s="46" t="s">
-        <v>169</v>
+      <c r="C29" s="45" t="s">
+        <v>172</v>
       </c>
       <c r="D29" s="13"/>
-      <c r="E29" s="47"/>
+      <c r="E29" s="46"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="47"/>
+      <c r="G29" s="46"/>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
-      <c r="M29" s="44"/>
+      <c r="M29" s="43"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37"/>
       <c r="B30" s="31"/>
-      <c r="C30" s="47"/>
+      <c r="C30" s="46"/>
       <c r="D30" s="13"/>
-      <c r="E30" s="47"/>
+      <c r="E30" s="46"/>
       <c r="F30" s="13"/>
-      <c r="G30" s="47"/>
+      <c r="G30" s="46"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
@@ -3557,89 +3156,89 @@
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="1:15" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="37">
         <v>0.58333333333333337</v>
       </c>
       <c r="B31" s="31"/>
-      <c r="C31" s="48"/>
+      <c r="C31" s="47"/>
       <c r="D31" s="13"/>
-      <c r="E31" s="48"/>
+      <c r="E31" s="47"/>
       <c r="F31" s="13"/>
-      <c r="G31" s="47"/>
+      <c r="G31" s="46"/>
       <c r="H31" s="13"/>
-      <c r="I31" s="46" t="s">
-        <v>183</v>
+      <c r="I31" s="45" t="s">
+        <v>187</v>
       </c>
       <c r="J31" s="13"/>
-      <c r="K31" s="46" t="s">
-        <v>187</v>
+      <c r="K31" s="45" t="s">
+        <v>191</v>
       </c>
       <c r="L31" s="13"/>
-      <c r="M31" s="42" t="s">
-        <v>148</v>
+      <c r="M31" s="41" t="s">
+        <v>149</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="37"/>
       <c r="B32" s="34"/>
       <c r="C32" s="33"/>
       <c r="D32" s="13"/>
       <c r="E32" s="33"/>
       <c r="F32" s="13"/>
-      <c r="G32" s="47"/>
+      <c r="G32" s="46"/>
       <c r="H32" s="13"/>
-      <c r="I32" s="47"/>
+      <c r="I32" s="46"/>
       <c r="J32" s="13"/>
-      <c r="K32" s="47"/>
+      <c r="K32" s="46"/>
       <c r="L32" s="13"/>
-      <c r="M32" s="43"/>
+      <c r="M32" s="42"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="1:15" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="37"/>
       <c r="B33" s="34"/>
-      <c r="C33" s="46" t="s">
-        <v>196</v>
+      <c r="C33" s="45" t="s">
+        <v>173</v>
       </c>
       <c r="D33" s="13"/>
-      <c r="E33" s="46" t="s">
-        <v>175</v>
+      <c r="E33" s="45" t="s">
+        <v>179</v>
       </c>
       <c r="F33" s="13"/>
-      <c r="G33" s="47"/>
+      <c r="G33" s="46"/>
       <c r="H33" s="13"/>
-      <c r="I33" s="47"/>
+      <c r="I33" s="46"/>
       <c r="J33" s="13"/>
-      <c r="K33" s="47"/>
+      <c r="K33" s="46"/>
       <c r="L33" s="13"/>
-      <c r="M33" s="43"/>
+      <c r="M33" s="42"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="1:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="37">
         <v>0.60416666666666663</v>
       </c>
       <c r="B34" s="34"/>
-      <c r="C34" s="48"/>
+      <c r="C34" s="47"/>
       <c r="D34" s="13"/>
-      <c r="E34" s="48"/>
+      <c r="E34" s="47"/>
       <c r="F34" s="13"/>
-      <c r="G34" s="48"/>
+      <c r="G34" s="47"/>
       <c r="H34" s="13"/>
-      <c r="I34" s="48"/>
+      <c r="I34" s="47"/>
       <c r="J34" s="13"/>
-      <c r="K34" s="48"/>
+      <c r="K34" s="47"/>
       <c r="L34" s="13"/>
-      <c r="M34" s="43"/>
+      <c r="M34" s="42"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="37"/>
       <c r="B35" s="34"/>
       <c r="C35" s="36"/>
@@ -3652,526 +3251,526 @@
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
-      <c r="M35" s="43"/>
+      <c r="M35" s="42"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
     </row>
-    <row r="36" spans="1:15" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="37"/>
       <c r="B36" s="34"/>
-      <c r="C36" s="46" t="s">
-        <v>170</v>
+      <c r="C36" s="45" t="s">
+        <v>174</v>
       </c>
       <c r="D36" s="13"/>
-      <c r="E36" s="46" t="s">
-        <v>176</v>
+      <c r="E36" s="45" t="s">
+        <v>180</v>
       </c>
       <c r="F36" s="13"/>
-      <c r="G36" s="46" t="s">
-        <v>181</v>
+      <c r="G36" s="45" t="s">
+        <v>185</v>
       </c>
       <c r="H36" s="13"/>
-      <c r="I36" s="46" t="s">
-        <v>184</v>
-      </c>
-      <c r="J36" s="45"/>
-      <c r="K36" s="46" t="s">
+      <c r="I36" s="45" t="s">
         <v>188</v>
       </c>
+      <c r="J36" s="44"/>
+      <c r="K36" s="45" t="s">
+        <v>192</v>
+      </c>
       <c r="L36" s="13"/>
-      <c r="M36" s="44"/>
+      <c r="M36" s="43"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="37"/>
       <c r="B37" s="34"/>
-      <c r="C37" s="47"/>
+      <c r="C37" s="46"/>
       <c r="D37" s="13"/>
-      <c r="E37" s="47"/>
+      <c r="E37" s="46"/>
       <c r="F37" s="13"/>
-      <c r="G37" s="47"/>
+      <c r="G37" s="46"/>
       <c r="H37" s="13"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="47"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="46"/>
       <c r="L37" s="13"/>
       <c r="M37" s="13"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="1:15" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="37">
         <v>0.625</v>
       </c>
       <c r="B38" s="34"/>
-      <c r="C38" s="48"/>
+      <c r="C38" s="47"/>
       <c r="D38" s="13"/>
-      <c r="E38" s="48"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="13"/>
-      <c r="G38" s="47"/>
+      <c r="G38" s="46"/>
       <c r="H38" s="13"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="47"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="46"/>
       <c r="L38" s="13"/>
-      <c r="M38" s="42" t="s">
-        <v>147</v>
+      <c r="M38" s="41" t="s">
+        <v>148</v>
       </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="37"/>
       <c r="B39" s="34"/>
       <c r="C39" s="33"/>
-      <c r="D39" s="45"/>
+      <c r="D39" s="44"/>
       <c r="E39" s="33"/>
       <c r="F39" s="13"/>
-      <c r="G39" s="47"/>
+      <c r="G39" s="46"/>
       <c r="H39" s="13"/>
-      <c r="I39" s="47"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="47"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="46"/>
       <c r="L39" s="13"/>
-      <c r="M39" s="43"/>
+      <c r="M39" s="42"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37"/>
       <c r="B40" s="34"/>
-      <c r="C40" s="46" t="s">
-        <v>171</v>
-      </c>
-      <c r="D40" s="45"/>
-      <c r="E40" s="46" t="s">
-        <v>177</v>
+      <c r="C40" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="D40" s="44"/>
+      <c r="E40" s="45" t="s">
+        <v>181</v>
       </c>
       <c r="F40" s="13"/>
-      <c r="G40" s="47"/>
+      <c r="G40" s="46"/>
       <c r="H40" s="13"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="48"/>
+      <c r="I40" s="47"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="47"/>
       <c r="L40" s="13"/>
-      <c r="M40" s="43"/>
+      <c r="M40" s="42"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
     </row>
-    <row r="41" spans="1:15" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="37">
         <v>0.64583333333333337</v>
       </c>
       <c r="B41" s="34"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="47"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="46"/>
       <c r="F41" s="13"/>
-      <c r="G41" s="47"/>
+      <c r="G41" s="46"/>
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
-      <c r="J41" s="45"/>
+      <c r="J41" s="44"/>
       <c r="K41" s="13"/>
       <c r="L41" s="13"/>
-      <c r="M41" s="43"/>
+      <c r="M41" s="42"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
     </row>
-    <row r="42" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="37"/>
       <c r="B42" s="34"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="48"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="47"/>
       <c r="F42" s="13"/>
-      <c r="G42" s="47"/>
+      <c r="G42" s="46"/>
       <c r="H42" s="13"/>
-      <c r="I42" s="46" t="s">
-        <v>185</v>
-      </c>
-      <c r="J42" s="45"/>
-      <c r="K42" s="46" t="s">
+      <c r="I42" s="45" t="s">
         <v>189</v>
       </c>
+      <c r="J42" s="44"/>
+      <c r="K42" s="45" t="s">
+        <v>193</v>
+      </c>
       <c r="L42" s="13"/>
-      <c r="M42" s="43"/>
+      <c r="M42" s="42"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="37"/>
       <c r="B43" s="34"/>
       <c r="C43" s="32"/>
       <c r="D43" s="13"/>
       <c r="E43" s="33"/>
       <c r="F43" s="13"/>
-      <c r="G43" s="48"/>
+      <c r="G43" s="47"/>
       <c r="H43" s="13"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="45"/>
-      <c r="K43" s="47"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="46"/>
       <c r="L43" s="13"/>
-      <c r="M43" s="43"/>
+      <c r="M43" s="42"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
     </row>
-    <row r="44" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="37"/>
       <c r="B44" s="34"/>
-      <c r="C44" s="46" t="s">
-        <v>193</v>
+      <c r="C44" s="45" t="s">
+        <v>197</v>
       </c>
       <c r="D44" s="13"/>
-      <c r="E44" s="46" t="s">
-        <v>178</v>
+      <c r="E44" s="45" t="s">
+        <v>182</v>
       </c>
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
-      <c r="I44" s="47"/>
-      <c r="J44" s="45"/>
-      <c r="K44" s="47"/>
+      <c r="I44" s="46"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="46"/>
       <c r="L44" s="13"/>
-      <c r="M44" s="44"/>
+      <c r="M44" s="43"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
     </row>
-    <row r="45" spans="1:15" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="37">
         <v>0.66666666666666663</v>
       </c>
       <c r="B45" s="34"/>
-      <c r="C45" s="47"/>
+      <c r="C45" s="46"/>
       <c r="D45" s="13"/>
-      <c r="E45" s="47"/>
+      <c r="E45" s="46"/>
       <c r="F45" s="13"/>
-      <c r="G45" s="46" t="s">
-        <v>182</v>
+      <c r="G45" s="45" t="s">
+        <v>186</v>
       </c>
       <c r="H45" s="13"/>
-      <c r="I45" s="47"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="47"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="46"/>
       <c r="L45" s="13"/>
       <c r="M45" s="13"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="37"/>
       <c r="B46" s="34"/>
-      <c r="C46" s="47"/>
+      <c r="C46" s="46"/>
       <c r="D46" s="13"/>
-      <c r="E46" s="47"/>
+      <c r="E46" s="46"/>
       <c r="F46" s="13"/>
-      <c r="G46" s="47"/>
+      <c r="G46" s="46"/>
       <c r="H46" s="13"/>
-      <c r="I46" s="47"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="47"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="46"/>
       <c r="L46" s="13"/>
-      <c r="M46" s="42" t="s">
-        <v>146</v>
+      <c r="M46" s="41" t="s">
+        <v>147</v>
       </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="37"/>
       <c r="B47" s="34"/>
-      <c r="C47" s="47"/>
+      <c r="C47" s="46"/>
       <c r="D47" s="13"/>
-      <c r="E47" s="47"/>
+      <c r="E47" s="46"/>
       <c r="F47" s="13"/>
-      <c r="G47" s="47"/>
+      <c r="G47" s="46"/>
       <c r="H47" s="13"/>
-      <c r="I47" s="48"/>
-      <c r="J47" s="45"/>
-      <c r="K47" s="48"/>
+      <c r="I47" s="47"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="47"/>
       <c r="L47" s="13"/>
-      <c r="M47" s="43"/>
+      <c r="M47" s="42"/>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
     </row>
-    <row r="48" spans="1:15" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="37"/>
       <c r="B48" s="34"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="48"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="47"/>
       <c r="F48" s="13"/>
-      <c r="G48" s="47"/>
+      <c r="G48" s="46"/>
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
       <c r="K48" s="13"/>
       <c r="L48" s="13"/>
-      <c r="M48" s="43"/>
+      <c r="M48" s="42"/>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
     </row>
-    <row r="49" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="37"/>
       <c r="B49" s="34"/>
       <c r="C49" s="32"/>
-      <c r="D49" s="45"/>
+      <c r="D49" s="44"/>
       <c r="E49" s="33"/>
       <c r="F49" s="13"/>
-      <c r="G49" s="47"/>
+      <c r="G49" s="46"/>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
       <c r="K49" s="13"/>
       <c r="L49" s="13"/>
-      <c r="M49" s="43"/>
+      <c r="M49" s="42"/>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
     </row>
-    <row r="50" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="37">
         <v>0.6875</v>
       </c>
       <c r="B50" s="34"/>
-      <c r="C50" s="46" t="s">
-        <v>172</v>
-      </c>
-      <c r="D50" s="45"/>
-      <c r="E50" s="46" t="s">
-        <v>179</v>
+      <c r="C50" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="D50" s="44"/>
+      <c r="E50" s="45" t="s">
+        <v>183</v>
       </c>
       <c r="F50" s="13"/>
-      <c r="G50" s="47"/>
+      <c r="G50" s="46"/>
       <c r="H50" s="13"/>
-      <c r="I50" s="46" t="s">
-        <v>186</v>
+      <c r="I50" s="45" t="s">
+        <v>190</v>
       </c>
       <c r="J50" s="13"/>
-      <c r="K50" s="46" t="s">
-        <v>190</v>
+      <c r="K50" s="45" t="s">
+        <v>194</v>
       </c>
       <c r="L50" s="13"/>
-      <c r="M50" s="43"/>
+      <c r="M50" s="42"/>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
     </row>
-    <row r="51" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="37"/>
       <c r="B51" s="34"/>
-      <c r="C51" s="47"/>
+      <c r="C51" s="46"/>
       <c r="D51" s="13"/>
-      <c r="E51" s="47"/>
+      <c r="E51" s="46"/>
       <c r="F51" s="13"/>
-      <c r="G51" s="47"/>
+      <c r="G51" s="46"/>
       <c r="H51" s="13"/>
-      <c r="I51" s="47"/>
+      <c r="I51" s="46"/>
       <c r="J51" s="13"/>
-      <c r="K51" s="47"/>
+      <c r="K51" s="46"/>
       <c r="L51" s="13"/>
-      <c r="M51" s="43"/>
+      <c r="M51" s="42"/>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
     </row>
-    <row r="52" spans="1:15" ht="10.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" ht="10.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="37"/>
       <c r="B52" s="34"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="47"/>
+      <c r="C52" s="46"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="46"/>
       <c r="F52" s="13"/>
-      <c r="G52" s="47"/>
+      <c r="G52" s="46"/>
       <c r="H52" s="13"/>
-      <c r="I52" s="47"/>
-      <c r="J52" s="45"/>
-      <c r="K52" s="47"/>
+      <c r="I52" s="46"/>
+      <c r="J52" s="44"/>
+      <c r="K52" s="46"/>
       <c r="L52" s="13"/>
-      <c r="M52" s="43"/>
+      <c r="M52" s="42"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="37"/>
       <c r="B53" s="34"/>
-      <c r="C53" s="47"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="47"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="46"/>
       <c r="F53" s="13"/>
-      <c r="G53" s="47"/>
+      <c r="G53" s="46"/>
       <c r="H53" s="13"/>
-      <c r="I53" s="47"/>
-      <c r="J53" s="45"/>
-      <c r="K53" s="47"/>
+      <c r="I53" s="46"/>
+      <c r="J53" s="44"/>
+      <c r="K53" s="46"/>
       <c r="L53" s="13"/>
-      <c r="M53" s="43"/>
+      <c r="M53" s="42"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
     </row>
-    <row r="54" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="37">
         <v>0.70833333333333337</v>
       </c>
       <c r="B54" s="34"/>
-      <c r="C54" s="47"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="47"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="46"/>
       <c r="F54" s="13"/>
-      <c r="G54" s="48"/>
+      <c r="G54" s="47"/>
       <c r="H54" s="13"/>
-      <c r="I54" s="47"/>
-      <c r="J54" s="45"/>
-      <c r="K54" s="47"/>
+      <c r="I54" s="46"/>
+      <c r="J54" s="44"/>
+      <c r="K54" s="46"/>
       <c r="L54" s="13"/>
-      <c r="M54" s="44"/>
+      <c r="M54" s="43"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
     </row>
-    <row r="55" spans="1:15" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="37"/>
       <c r="B55" s="34"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="47"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="46"/>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
-      <c r="I55" s="47"/>
-      <c r="J55" s="45"/>
-      <c r="K55" s="47"/>
+      <c r="I55" s="46"/>
+      <c r="J55" s="44"/>
+      <c r="K55" s="46"/>
       <c r="L55" s="13"/>
       <c r="M55" s="13"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
     </row>
-    <row r="56" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="37"/>
       <c r="B56" s="34"/>
-      <c r="C56" s="47"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="47"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="44"/>
+      <c r="E56" s="46"/>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
-      <c r="I56" s="48"/>
-      <c r="J56" s="45"/>
-      <c r="K56" s="48"/>
+      <c r="I56" s="47"/>
+      <c r="J56" s="44"/>
+      <c r="K56" s="47"/>
       <c r="L56" s="13"/>
-      <c r="M56" s="42" t="s">
-        <v>141</v>
+      <c r="M56" s="41" t="s">
+        <v>142</v>
       </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
     </row>
-    <row r="57" spans="1:15" ht="10.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" ht="10.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="37"/>
       <c r="B57" s="34"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="48"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="47"/>
       <c r="F57" s="13"/>
-      <c r="G57" s="46" t="s">
-        <v>155</v>
+      <c r="G57" s="45" t="s">
+        <v>157</v>
       </c>
       <c r="H57" s="13"/>
       <c r="I57" s="13"/>
-      <c r="J57" s="45"/>
+      <c r="J57" s="44"/>
       <c r="K57" s="13"/>
       <c r="L57" s="13"/>
-      <c r="M57" s="43"/>
+      <c r="M57" s="42"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
     </row>
-    <row r="58" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="37"/>
       <c r="B58" s="34"/>
       <c r="C58" s="33"/>
-      <c r="D58" s="45"/>
+      <c r="D58" s="44"/>
       <c r="E58" s="33"/>
       <c r="F58" s="13"/>
-      <c r="G58" s="47"/>
+      <c r="G58" s="46"/>
       <c r="H58" s="13"/>
-      <c r="I58" s="46" t="s">
-        <v>194</v>
-      </c>
-      <c r="J58" s="45"/>
-      <c r="K58" s="46" t="s">
-        <v>142</v>
+      <c r="I58" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="J58" s="44"/>
+      <c r="K58" s="45" t="s">
+        <v>143</v>
       </c>
       <c r="L58" s="13"/>
-      <c r="M58" s="43"/>
+      <c r="M58" s="42"/>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
     </row>
-    <row r="59" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="37">
         <v>0.72916666666666663</v>
       </c>
       <c r="B59" s="34"/>
-      <c r="C59" s="46" t="s">
-        <v>173</v>
-      </c>
-      <c r="D59" s="45"/>
-      <c r="E59" s="46" t="s">
-        <v>145</v>
+      <c r="C59" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="D59" s="44"/>
+      <c r="E59" s="45" t="s">
+        <v>146</v>
       </c>
       <c r="F59" s="13"/>
-      <c r="G59" s="47"/>
+      <c r="G59" s="46"/>
       <c r="H59" s="13"/>
-      <c r="I59" s="47"/>
-      <c r="J59" s="45"/>
-      <c r="K59" s="47"/>
+      <c r="I59" s="46"/>
+      <c r="J59" s="44"/>
+      <c r="K59" s="46"/>
       <c r="L59" s="13"/>
-      <c r="M59" s="43"/>
+      <c r="M59" s="42"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
     </row>
-    <row r="60" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="37"/>
       <c r="B60" s="34"/>
-      <c r="C60" s="48"/>
+      <c r="C60" s="47"/>
       <c r="D60" s="13"/>
-      <c r="E60" s="48"/>
+      <c r="E60" s="47"/>
       <c r="F60" s="13"/>
-      <c r="G60" s="47"/>
+      <c r="G60" s="46"/>
       <c r="H60" s="13"/>
-      <c r="I60" s="47"/>
+      <c r="I60" s="46"/>
       <c r="J60" s="13"/>
-      <c r="K60" s="47"/>
+      <c r="K60" s="46"/>
       <c r="L60" s="13"/>
-      <c r="M60" s="43"/>
+      <c r="M60" s="42"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
     </row>
-    <row r="61" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="37"/>
       <c r="B61" s="34"/>
       <c r="C61" s="33"/>
       <c r="D61" s="13"/>
       <c r="E61" s="33"/>
       <c r="F61" s="13"/>
-      <c r="G61" s="47"/>
+      <c r="G61" s="46"/>
       <c r="H61" s="13"/>
-      <c r="I61" s="48"/>
+      <c r="I61" s="47"/>
       <c r="J61" s="13"/>
-      <c r="K61" s="48"/>
+      <c r="K61" s="47"/>
       <c r="L61" s="13"/>
-      <c r="M61" s="44"/>
+      <c r="M61" s="43"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
     </row>
-    <row r="62" spans="1:15" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="37">
         <v>0.75</v>
       </c>
       <c r="B62" s="34"/>
-      <c r="C62" s="46" t="s">
-        <v>192</v>
+      <c r="C62" s="45" t="s">
+        <v>196</v>
       </c>
       <c r="D62" s="13"/>
-      <c r="E62" s="46" t="s">
-        <v>191</v>
+      <c r="E62" s="45" t="s">
+        <v>195</v>
       </c>
       <c r="F62" s="13"/>
-      <c r="G62" s="48"/>
+      <c r="G62" s="47"/>
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
       <c r="J62" s="13"/>
@@ -4181,130 +3780,130 @@
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
     </row>
-    <row r="63" spans="1:15" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="37"/>
       <c r="B63" s="34"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="45"/>
-      <c r="E63" s="48"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="47"/>
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
-      <c r="J63" s="45"/>
+      <c r="J63" s="44"/>
       <c r="K63" s="13"/>
       <c r="L63" s="13"/>
       <c r="M63" s="13"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
     </row>
-    <row r="64" spans="1:15" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="37"/>
       <c r="B64" s="34"/>
       <c r="C64" s="33"/>
-      <c r="D64" s="45"/>
+      <c r="D64" s="44"/>
       <c r="E64" s="33"/>
       <c r="F64" s="13"/>
       <c r="G64" s="13"/>
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
-      <c r="J64" s="45"/>
+      <c r="J64" s="44"/>
       <c r="K64" s="13"/>
       <c r="L64" s="13"/>
       <c r="M64" s="13"/>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
     </row>
-    <row r="65" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="37">
         <v>0.77083333333333337</v>
       </c>
       <c r="B65" s="34"/>
       <c r="C65" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="D65" s="45"/>
+        <v>141</v>
+      </c>
+      <c r="D65" s="44"/>
       <c r="E65" s="33"/>
       <c r="F65" s="13"/>
       <c r="G65" s="13"/>
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
-      <c r="J65" s="45"/>
+      <c r="J65" s="44"/>
       <c r="K65" s="13"/>
       <c r="L65" s="13"/>
       <c r="M65" s="13"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
     </row>
-    <row r="66" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="37"/>
       <c r="B66" s="34"/>
       <c r="C66" s="33"/>
-      <c r="D66" s="45"/>
+      <c r="D66" s="44"/>
       <c r="E66" s="33"/>
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
-      <c r="J66" s="45"/>
+      <c r="J66" s="44"/>
       <c r="K66" s="13"/>
       <c r="L66" s="13"/>
       <c r="M66" s="13"/>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
     </row>
-    <row r="67" spans="1:15" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="37"/>
       <c r="B67" s="34"/>
       <c r="C67" s="33"/>
-      <c r="D67" s="45"/>
+      <c r="D67" s="44"/>
       <c r="E67" s="33"/>
       <c r="F67" s="13"/>
       <c r="G67" s="13"/>
       <c r="H67" s="13"/>
       <c r="I67" s="13"/>
-      <c r="J67" s="45"/>
+      <c r="J67" s="44"/>
       <c r="K67" s="13"/>
       <c r="L67" s="13"/>
       <c r="M67" s="13"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
     </row>
-    <row r="68" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="30"/>
       <c r="B68" s="34"/>
       <c r="C68" s="33"/>
-      <c r="D68" s="45"/>
+      <c r="D68" s="44"/>
       <c r="E68" s="33"/>
       <c r="F68" s="13"/>
       <c r="G68" s="13"/>
       <c r="H68" s="13"/>
       <c r="I68" s="13"/>
-      <c r="J68" s="45"/>
+      <c r="J68" s="44"/>
       <c r="K68" s="13"/>
       <c r="L68" s="13"/>
       <c r="M68" s="13"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
     </row>
-    <row r="69" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="30"/>
       <c r="B69" s="34"/>
       <c r="C69" s="33"/>
-      <c r="D69" s="45"/>
+      <c r="D69" s="44"/>
       <c r="E69" s="33"/>
       <c r="F69" s="13"/>
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
-      <c r="J69" s="45"/>
+      <c r="J69" s="44"/>
       <c r="K69" s="13"/>
       <c r="L69" s="13"/>
       <c r="M69" s="13"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
     </row>
-    <row r="70" spans="1:15" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="24"/>
       <c r="B70" s="1"/>
       <c r="C70" s="20"/>
@@ -4321,7 +3920,7 @@
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
     </row>
-    <row r="71" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="24"/>
       <c r="B71" s="1"/>
       <c r="C71" s="18"/>
@@ -4338,7 +3937,7 @@
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
     </row>
-    <row r="72" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="24"/>
       <c r="B72" s="1"/>
       <c r="C72" s="18"/>
@@ -4355,109 +3954,109 @@
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
     </row>
-    <row r="73" spans="1:15" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="24"/>
       <c r="B73" s="1"/>
       <c r="C73" s="23"/>
-      <c r="D73" s="45"/>
+      <c r="D73" s="44"/>
       <c r="E73" s="23"/>
       <c r="F73" s="1"/>
       <c r="G73" s="6"/>
       <c r="H73" s="1"/>
       <c r="I73" s="6"/>
-      <c r="J73" s="45"/>
+      <c r="J73" s="44"/>
       <c r="K73" s="6"/>
       <c r="L73" s="1"/>
       <c r="M73" s="6"/>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
     </row>
-    <row r="74" spans="1:15" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="24"/>
       <c r="B74" s="1"/>
       <c r="C74" s="23"/>
-      <c r="D74" s="45"/>
+      <c r="D74" s="44"/>
       <c r="E74" s="23"/>
       <c r="F74" s="1"/>
       <c r="G74" s="6"/>
       <c r="H74" s="1"/>
       <c r="I74" s="6"/>
-      <c r="J74" s="45"/>
+      <c r="J74" s="44"/>
       <c r="K74" s="6"/>
       <c r="L74" s="1"/>
       <c r="M74" s="6"/>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
     </row>
-    <row r="75" spans="1:15" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="24"/>
       <c r="B75" s="1"/>
       <c r="C75" s="23"/>
-      <c r="D75" s="45"/>
+      <c r="D75" s="44"/>
       <c r="E75" s="23"/>
       <c r="F75" s="1"/>
       <c r="G75" s="6"/>
       <c r="H75" s="1"/>
       <c r="I75" s="6"/>
-      <c r="J75" s="45"/>
+      <c r="J75" s="44"/>
       <c r="K75" s="6"/>
       <c r="L75" s="1"/>
       <c r="M75" s="6"/>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
     </row>
-    <row r="76" spans="1:15" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="24"/>
       <c r="B76" s="1"/>
       <c r="C76" s="23"/>
-      <c r="D76" s="45"/>
+      <c r="D76" s="44"/>
       <c r="E76" s="23"/>
       <c r="F76" s="1"/>
       <c r="G76" s="6"/>
       <c r="H76" s="1"/>
       <c r="I76" s="6"/>
-      <c r="J76" s="45"/>
+      <c r="J76" s="44"/>
       <c r="K76" s="6"/>
       <c r="L76" s="1"/>
       <c r="M76" s="6"/>
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="24"/>
       <c r="B77" s="1"/>
       <c r="C77" s="23"/>
-      <c r="D77" s="45"/>
+      <c r="D77" s="44"/>
       <c r="E77" s="23"/>
       <c r="F77" s="1"/>
       <c r="G77" s="6"/>
       <c r="H77" s="1"/>
       <c r="I77" s="6"/>
-      <c r="J77" s="45"/>
+      <c r="J77" s="44"/>
       <c r="K77" s="6"/>
       <c r="L77" s="1"/>
       <c r="M77" s="6"/>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
     </row>
-    <row r="78" spans="1:15" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="24"/>
       <c r="B78" s="1"/>
       <c r="C78" s="23"/>
-      <c r="D78" s="45"/>
+      <c r="D78" s="44"/>
       <c r="E78" s="23"/>
       <c r="F78" s="1"/>
       <c r="G78" s="6"/>
       <c r="H78" s="1"/>
       <c r="I78" s="6"/>
-      <c r="J78" s="45"/>
+      <c r="J78" s="44"/>
       <c r="K78" s="6"/>
       <c r="L78" s="1"/>
       <c r="M78" s="6"/>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
     </row>
-    <row r="79" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="24"/>
       <c r="B79" s="1"/>
       <c r="C79" s="18"/>
@@ -4467,14 +4066,14 @@
       <c r="G79" s="6"/>
       <c r="H79" s="1"/>
       <c r="I79" s="6"/>
-      <c r="J79" s="45"/>
+      <c r="J79" s="44"/>
       <c r="K79" s="6"/>
       <c r="L79" s="1"/>
       <c r="M79" s="6"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
     </row>
-    <row r="80" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="24"/>
       <c r="B80" s="1"/>
       <c r="C80" s="18"/>
@@ -4484,69 +4083,69 @@
       <c r="G80" s="6"/>
       <c r="H80" s="1"/>
       <c r="I80" s="6"/>
-      <c r="J80" s="45"/>
+      <c r="J80" s="44"/>
       <c r="K80" s="6"/>
       <c r="L80" s="1"/>
       <c r="M80" s="6"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
     </row>
-    <row r="81" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="24"/>
       <c r="B81" s="1"/>
       <c r="C81" s="23"/>
-      <c r="D81" s="45"/>
+      <c r="D81" s="44"/>
       <c r="E81" s="23"/>
       <c r="F81" s="1"/>
       <c r="G81" s="6"/>
       <c r="H81" s="1"/>
       <c r="I81" s="6"/>
-      <c r="J81" s="45"/>
+      <c r="J81" s="44"/>
       <c r="K81" s="6"/>
       <c r="L81" s="1"/>
       <c r="M81" s="6"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
     </row>
-    <row r="82" spans="1:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="24"/>
       <c r="B82" s="1"/>
       <c r="C82" s="23"/>
-      <c r="D82" s="45"/>
+      <c r="D82" s="44"/>
       <c r="E82" s="23"/>
       <c r="F82" s="1"/>
       <c r="G82" s="6"/>
       <c r="H82" s="1"/>
       <c r="I82" s="6"/>
-      <c r="J82" s="45"/>
+      <c r="J82" s="44"/>
       <c r="K82" s="6"/>
       <c r="L82" s="1"/>
       <c r="M82" s="6"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
     </row>
-    <row r="83" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="24"/>
       <c r="B83" s="1"/>
       <c r="C83" s="23"/>
-      <c r="D83" s="45"/>
+      <c r="D83" s="44"/>
       <c r="E83" s="23"/>
       <c r="F83" s="1"/>
       <c r="G83" s="6"/>
       <c r="H83" s="1"/>
       <c r="I83" s="6"/>
-      <c r="J83" s="45"/>
+      <c r="J83" s="44"/>
       <c r="K83" s="6"/>
       <c r="L83" s="1"/>
       <c r="M83" s="6"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" s="24"/>
       <c r="B84" s="1"/>
       <c r="C84" s="23"/>
-      <c r="D84" s="45"/>
+      <c r="D84" s="44"/>
       <c r="E84" s="23"/>
       <c r="F84" s="1"/>
       <c r="G84" s="6"/>
@@ -4559,7 +4158,7 @@
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
     </row>
-    <row r="85" spans="1:15" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="24"/>
       <c r="B85" s="1"/>
       <c r="C85" s="7"/>
@@ -4576,53 +4175,53 @@
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
     </row>
-    <row r="86" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="27"/>
     </row>
-    <row r="87" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="27"/>
     </row>
-    <row r="88" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="27"/>
     </row>
-    <row r="89" spans="1:15" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="27"/>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" s="27"/>
     </row>
-    <row r="91" spans="1:15" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="27"/>
     </row>
-    <row r="92" spans="1:15" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="27"/>
     </row>
-    <row r="93" spans="1:15" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="27"/>
     </row>
-    <row r="94" spans="1:15" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="27"/>
     </row>
-    <row r="95" spans="1:15" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="27"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="27"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="27"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="27"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="27"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="55"/>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="55"/>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="54"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="76">
@@ -4644,10 +4243,10 @@
     <mergeCell ref="K36:K40"/>
     <mergeCell ref="K16:K19"/>
     <mergeCell ref="K21:K25"/>
+    <mergeCell ref="M13:M17"/>
     <mergeCell ref="M19:M22"/>
+    <mergeCell ref="M7:M11"/>
     <mergeCell ref="M24:M29"/>
-    <mergeCell ref="M14:M18"/>
-    <mergeCell ref="M10:M13"/>
     <mergeCell ref="C36:C38"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="E10:E13"/>
@@ -4757,9 +4356,6 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
-  <customProperties>
-    <customPr name="_pios_id" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
 
@@ -4770,23 +4366,23 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1"/>
-    <col min="6" max="6" width="41.5546875" customWidth="1"/>
-    <col min="7" max="7" width="88.109375" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" customWidth="1"/>
+    <col min="7" max="7" width="88.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>8</v>
@@ -4810,7 +4406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>0.41666666666666669</v>
       </c>
@@ -4821,22 +4417,22 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="225" x14ac:dyDescent="0.25">
       <c r="B3" s="11">
         <v>0.44444444444444442</v>
       </c>
@@ -4844,22 +4440,22 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="B4" s="11">
         <v>0.44444444444444442</v>
       </c>
@@ -4867,22 +4463,22 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="11">
         <v>0.4513888888888889</v>
       </c>
@@ -4896,16 +4492,16 @@
         <v>21</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="11">
         <v>0.4513888888888889</v>
       </c>
@@ -4916,17 +4512,17 @@
         <v>12</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>0.45833333333333331</v>
       </c>
@@ -4937,22 +4533,22 @@
         <v>0.50694444444444442</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <v>0.47916666666666669</v>
       </c>
@@ -4960,22 +4556,22 @@
         <v>0.50694444444444442</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H8" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B9" s="11">
         <v>0.4861111111111111</v>
       </c>
@@ -4989,16 +4585,16 @@
         <v>32</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="11">
         <v>0.4861111111111111</v>
       </c>
@@ -5009,17 +4605,17 @@
         <v>12</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>0.5</v>
       </c>
@@ -5030,22 +4626,22 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
         <v>0.51388888888888895</v>
       </c>
@@ -5053,22 +4649,22 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <v>0.52083333333333337</v>
       </c>
@@ -5082,16 +4678,16 @@
         <v>24</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
         <v>0.52083333333333337</v>
       </c>
@@ -5105,16 +4701,16 @@
         <v>27</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
         <v>0.54166666666666663</v>
       </c>
@@ -5125,22 +4721,22 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H15" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
         <v>0.5625</v>
       </c>
@@ -5148,20 +4744,20 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>0.56944444444444442</v>
       </c>
@@ -5169,22 +4765,22 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
         <v>0.58333333333333337</v>
       </c>
@@ -5198,16 +4794,16 @@
         <v>30</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>0.58333333333333337</v>
       </c>
@@ -5221,17 +4817,17 @@
         <v>12</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
         <v>0.59722222222222221</v>
       </c>
@@ -5239,20 +4835,20 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>23</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
         <v>0.59722222222222221</v>
       </c>
@@ -5260,20 +4856,20 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>199</v>
+        <v>34</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H21" s="12"/>
     </row>
-    <row r="22" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <v>0.61805555555555558</v>
       </c>
@@ -5281,22 +4877,22 @@
         <v>0.65972222222222221</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
         <v>0.61805555555555558</v>
       </c>
@@ -5307,19 +4903,19 @@
         <v>11</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
         <v>0.61805555555555558</v>
       </c>
@@ -5327,22 +4923,22 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>0.625</v>
       </c>
@@ -5353,20 +4949,20 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H25" s="12"/>
     </row>
-    <row r="26" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
         <v>0.63888888888888895</v>
       </c>
@@ -5374,20 +4970,20 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>33</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H26" s="12"/>
     </row>
-    <row r="27" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
         <v>0.65277777777777779</v>
       </c>
@@ -5398,19 +4994,19 @@
         <v>12</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
         <v>0.65277777777777779</v>
       </c>
@@ -5421,19 +5017,19 @@
         <v>11</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
         <v>0.65972222222222221</v>
       </c>
@@ -5441,22 +5037,22 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>20</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
         <v>0.65972222222222221</v>
       </c>
@@ -5464,22 +5060,22 @@
         <v>0.6875</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
         <v>0.65972222222222221</v>
       </c>
@@ -5487,22 +5083,22 @@
         <v>0.6875</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H31" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>0.66666666666666663</v>
       </c>
@@ -5513,22 +5109,22 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
         <v>0.6875</v>
       </c>
@@ -5539,19 +5135,19 @@
         <v>11</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
         <v>0.6875</v>
       </c>
@@ -5562,19 +5158,19 @@
         <v>12</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
         <v>0.69444444444444453</v>
       </c>
@@ -5582,22 +5178,22 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
         <v>0.70138888888888884</v>
       </c>
@@ -5605,22 +5201,22 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H36" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>0.70833333333333337</v>
       </c>
@@ -5631,22 +5227,22 @@
         <v>0.75694444444444453</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>28</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
         <v>0.72222222222222221</v>
       </c>
@@ -5657,17 +5253,17 @@
         <v>11</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G38" s="9"/>
       <c r="H38" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
         <v>0.72916666666666663</v>
       </c>
@@ -5675,22 +5271,22 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B40" s="11">
         <v>0.72916666666666663</v>
       </c>
@@ -5698,22 +5294,22 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="D40" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H40" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="E40" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H40" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>0.75</v>
       </c>
@@ -5724,22 +5320,22 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B42" s="11">
         <v>0.75</v>
       </c>
@@ -5747,25 +5343,25 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="D42" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H42" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="E42" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="H42" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G43" s="9"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G44" s="9"/>
     </row>
   </sheetData>
@@ -5774,8 +5370,5 @@
   </sortState>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="48" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <customProperties>
-    <customPr name="_pios_id" r:id="rId2"/>
-  </customProperties>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UI5Con Agenda Update 27.6.2017 15:30
</commit_message>
<xml_diff>
--- a/ui5con/downloads/ui5con_2017_agenda.xlsx
+++ b/ui5con/downloads/ui5con_2017_agenda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d068664\Documents\20170620 UI5Con\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d068664\WebstormProjects\ui5con\src\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Details" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agenda UI5con@SAP'!$A$1:$O$113</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Details!$A$1:$G$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agenda UI5con@SAP'!$A$1:$O$114</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Details!$A$1:$G$57</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Details!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="219">
   <si>
     <r>
       <rPr>
@@ -114,9 +114,6 @@
     <t>Jan Zaruba, Tomas Krejci</t>
   </si>
   <si>
-    <t>17:10 - 18:10</t>
-  </si>
-  <si>
     <t>Frederic Berg</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>16:00 - 17:00</t>
   </si>
   <si>
-    <t>16:20 - 17:00</t>
-  </si>
-  <si>
     <t>Christoph Laux</t>
   </si>
   <si>
@@ -192,9 +186,6 @@
     <t>Mateusz Skadorwa, Tomasz Wilk</t>
   </si>
   <si>
-    <t>15:30 - 16:10</t>
-  </si>
-  <si>
     <t>Integrate Feed Capabilities Using UI5 Controls</t>
   </si>
   <si>
@@ -246,9 +237,6 @@
     <t>Building a companion conversational UI for a Fiori App</t>
   </si>
   <si>
-    <t>14:40 - 15:20</t>
-  </si>
-  <si>
     <t>Vered Constantin</t>
   </si>
   <si>
@@ -303,15 +291,9 @@
     <t>Michael Graf, Emanuele Ricci</t>
   </si>
   <si>
-    <t>13:50 - 14:30</t>
-  </si>
-  <si>
     <t>Stephan Heyne</t>
   </si>
   <si>
-    <t>Peter Muessig, Matthias Osswal</t>
-  </si>
-  <si>
     <t>The UI5 app to create UI5 apps</t>
   </si>
   <si>
@@ -351,9 +333,6 @@
     <t>Functional Programming for your UI5 App</t>
   </si>
   <si>
-    <t>13:00 - 13:40</t>
-  </si>
-  <si>
     <t>Helmut Tammen</t>
   </si>
   <si>
@@ -417,9 +396,6 @@
     <t>HP Seitz</t>
   </si>
   <si>
-    <t>11:00 - 12:00</t>
-  </si>
-  <si>
     <t>Pia Kinkel, Bohdan Pukalskyi, Dominic Holzwarth</t>
   </si>
   <si>
@@ -462,9 +438,6 @@
     <t>Developer Clinic: UI5 Controls</t>
   </si>
   <si>
-    <t>10:20 - 11:00</t>
-  </si>
-  <si>
     <t>The OpenUI5 Developer Blog - Behind the Scenes</t>
   </si>
   <si>
@@ -492,9 +465,6 @@
     <t>Stefan Beck</t>
   </si>
   <si>
-    <t>09:40 - 10:20</t>
-  </si>
-  <si>
     <t>Pia Kinkel, Christoph Laux</t>
   </si>
   <si>
@@ -549,15 +519,9 @@
     <t>Session</t>
   </si>
   <si>
-    <t>All the news around UI5.</t>
-  </si>
-  <si>
     <t>Key Note</t>
   </si>
   <si>
-    <t>Demo new upcoming features of UI5 regarding Metadata Driven Controls.Allow to manipulate the artifacts live in an editor and see the immediate result.Create custom control using a Fragment Control, add a Swagger service to the View and enhance the metadata.Drive the new custom control and other UI controls from the metadata.</t>
-  </si>
-  <si>
     <t>Imagine a world where development and business can understand each other without using lengthy code lines. Applying human-readable language you will have the possibility to enable everyone in your team, even your customers, to create business driven automated tests.Our solution will lead your agile workflow towards acceptance testing using OPA5 and Cucumber over Fiori stack which provide basis for behavior driven development.We are going to present a Cucumber and OPA5-based test automation framework where users write test scenarios adopting human-readable Gherkin language. Additionally, we will talk about the key test concepts of healthy test automation pyramids, appropriate placement of test levels, and misconcepts about TDD and BDD.</t>
   </si>
   <si>
@@ -603,9 +567,6 @@
     <t>We will present newly released and upcoming controls which we have developed in Brno Suite Controls team. We will have prototypes and demos ready for the upcoming controls and demo apps for released controls. We’ll be happy to answer any questions regarding implementation of our controls in your apps.</t>
   </si>
   <si>
-    <t>Session Description: In this session we will write a custom component using OpenLayers v3 (http://www.openlayers.de) for showing a map. This map will be bound to a XMPPJsonPatchSyncModel (https://github.com/ManuelB/XMPPJSONPatchSyncModel) to make it possible to track other people in real time on the map.</t>
-  </si>
-  <si>
     <t>In our UI5 demo app, you'll learn to build an ice cream machine. We will show the demo app and a tutorial with a step-by-step explanation of how to build this app using various UI5 Controls.</t>
   </si>
   <si>
@@ -660,9 +621,6 @@
     <t>Session Description: In this session I will discuss options how UI5 web apps can be used as a basis for apps beyond your typical office requirements. While SAP Fiori apps and Fiori LaunchPad are the basis for SAPs Digital Workplace of the future, there exist much more possibilities how the web can be the basis for your digitalization efforts. We are looking into WebAPIs, standards such as WebRTC and 3rd party extensions and how this can be applied in enterprise settings. Adding Cloud APIs into the mix, lots of demand for feature-rich apps can already be fulfilled leveraging the web.</t>
   </si>
   <si>
-    <t>Let`s build a simple FLP plugin (based on a UI5 Component) together. Once deployed to a FLP on Cloud Platform we will start to use the renderer extension api of FLP to place SAPUI5 controls into the FLP UI to improve the user experience of the Lauchpad AND learn that SAPUI5 and Fiori Launchpad are actually of the same kind.</t>
-  </si>
-  <si>
     <t>Building a Conversational UI for the Fiori My Inbox app using API.AI. I will run through the code needed and do a live demo.</t>
   </si>
   <si>
@@ -681,9 +639,6 @@
     <t>Based on a public OpenUI5 boilerplate project (not published, yet) we want to share our experience and knowledge on how to setup and use a modern OpenUI5 app structure and build process by using Babel, Flow and Gulp (especially addressing non-SAP developers). Furthermore an overview of very useful best practices, does &amp; don'ts and quick enhancements (like new useful methods in the app Component and BaseController) that should speed up your development workflow and that keep the app maintainable and scalable.</t>
   </si>
   <si>
-    <t>Find out everything you need to know about the new version of SAP Fiori. Learn what makes Fiori 2.0 different and which are the new UI5 features empowering Fiori 2.0 experience.In this session we will show and tell how to develop your Fiori 2.0 app from scratch and even more - how to migrate your existing app to Fiori 2.0.</t>
-  </si>
-  <si>
     <t>Social media is ubiquitous, but a feed can also include system events or comments. UI5 provides a set of controls that support you in implementing feed capabilities for your application.</t>
   </si>
   <si>
@@ -699,9 +654,6 @@
     <t>What is SAP's new extensibility approach all about? Well, the key is flexibility. Partners and customers need to adapt the UIs of SAP apps, for example add, hide or rearrange fields. Sounds technical and complicated? SAPUI5 extensibility changes all that allowing upgrade-safe, modification-free, and role-based UI changes with intuitive and easy-to-use tools – even for non-developers.What's the strategy behind it, what are the benefits, and what's the roadmap? In this session you'll find out.</t>
   </si>
   <si>
-    <t>In this session, we will demonstrate how to get started on cloud foundry. We will see how to onboard onto the platform, install the necessary tools and deploy a UI5 application which makes use of platform services to persist its data.</t>
-  </si>
-  <si>
     <t>It all started with a Proof-of-Concept of a UI5 hybrid application for discrete object recognition on mobile devices. In the course of the PoC, research led to several experiments around the key words in the session title: from real-time Image manipulation via visual object recognition up to Augmented Reality flavors, all of that within the UI5 framework. I'd like to show the results of the experiments and evaluate their sustainability and production readiness.</t>
   </si>
   <si>
@@ -718,13 +670,70 @@
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>17:20 - 18:20</t>
+  </si>
+  <si>
+    <t>SAPUI5 is evolving and thus best practices or recommended controls change over time. In this session, you'll get an update on the new supportability tool, the new DemoKit, new and updated controls, news in the framework like our plans towards OData V4 and improved Smart Controls. Finally we'll share some insights into more radical renovation activities that will come early in 2018.</t>
+  </si>
+  <si>
+    <t>In this session we will use a custom component (https://github.com/ManuelB/openui5-ol/) that wraps the OpenLayers v3 API (http://www.openlayers.de) for showing a map. This map will be bound to a XMPPJsonPatchSyncModel (https://github.com/ManuelB/XMPPJSONPatchSyncModel) to make it possible to track other people in real time on the map.You should pre-install the following software on your notebook:  git  Your favorite IDE  ejabbered (a public server will be running on the speaker notebook)  A webserver e.g. (python -m SimpleHTTPServer 8000)</t>
+  </si>
+  <si>
+    <t>10:50 - 11:30</t>
+  </si>
+  <si>
+    <t>11:40 - 12:20</t>
+  </si>
+  <si>
+    <t>12:30 - 13:10</t>
+  </si>
+  <si>
+    <t>14:00 - 14:40</t>
+  </si>
+  <si>
+    <t>Peter Muessig, Matthias Oßwald</t>
+  </si>
+  <si>
+    <t>14:50 - 15:30</t>
+  </si>
+  <si>
+    <t>15:40 - 16:20</t>
+  </si>
+  <si>
+    <t>16:30 - 17:10</t>
+  </si>
+  <si>
+    <t>17:20 - 18:00</t>
+  </si>
+  <si>
+    <t>11:20 - 12:00</t>
+  </si>
+  <si>
+    <t>17:00 - 18:00</t>
+  </si>
+  <si>
+    <t>Concepts of upcoming features of UI5 to ease creation of building blocks and connection of controls to Rest Service Metadata.</t>
+  </si>
+  <si>
+    <t>Find out everything you need to know about the new version of SAP Fiori. Learn what makes Fiori 2.0 different and which are the new UI5 features empowering Fiori 2.0 experience.In this session we will show and tell how to develop your Fiori 2.0 app from scratch and even more - how to migrate your existing app to Fiori 2.0.Prerequisites:You will work in SAP WebIDE, trial accounts are already created for you, so you do not need anything else than your laptop. In case of network issues, we would fall back to using nodejs, NPM and Git, so you should preferably have those installed.</t>
+  </si>
+  <si>
+    <t>In this session, we will demonstrate how to get started on cloud foundry. We will see how to onboard onto the platform, install the necessary tools and deploy a UI5 application which makes use of platform services to persist its data.Prerequisites:Please have Node.js installed on your laptop and your own hanatrial account ready.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let's build a simple FLP plugin (based on a UI5 Component) together. Once deployed to a FLP on Cloud Platform we will start to use the renderer extension api of FLP to place SAPUI5 controls into the FLP UI to improve the user experience of the Lauchpad AND learn that SAPUI5 and Fiori Launchpad are actually of the same kind. Prerequisites:   - Laptop  - an SAP CP trial account </t>
+  </si>
+  <si>
+    <t>Last updated: 27.06.2017 14:55</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -808,6 +817,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFF26A36"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -896,7 +912,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -936,6 +952,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1255,8 +1284,8 @@
   </sheetPr>
   <dimension ref="A1:AB142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="A58" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114:C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,11 +1379,11 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="9" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="9" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -1362,17 +1391,11 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="N3" s="1"/>
       <c r="O3" s="6">
         <v>0.39583333333333331</v>
       </c>
@@ -1390,7 +1413,7 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="4" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>0.39930555555555558</v>
       </c>
@@ -1408,17 +1431,11 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="N4" s="1"/>
       <c r="O4" s="6">
         <v>0.39930555555555558</v>
       </c>
@@ -1442,11 +1459,11 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
@@ -1454,17 +1471,6 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="9" t="s">
-        <v>147</v>
-      </c>
       <c r="O5" s="6">
         <v>0.40277777777777801</v>
       </c>
@@ -1488,11 +1494,11 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="11" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="11" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
@@ -1500,17 +1506,6 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="O6" s="6">
         <v>0.40625</v>
       </c>
@@ -1534,11 +1529,11 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="9" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="9" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
@@ -1546,17 +1541,6 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="O7" s="6">
         <v>0.40972222222222199</v>
       </c>
@@ -1592,17 +1576,6 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="O8" s="6">
         <v>0.41319444444444497</v>
       </c>
@@ -1638,17 +1611,6 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="O9" s="6">
         <v>0.41666666666666702</v>
       </c>
@@ -1684,17 +1646,6 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="1"/>
-      <c r="L10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="1"/>
-      <c r="N10" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="O10" s="6">
         <v>0.42013888888888901</v>
       </c>
@@ -1730,17 +1681,6 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="10" t="s">
-        <v>141</v>
-      </c>
       <c r="O11" s="6">
         <v>0.42361111111111099</v>
       </c>
@@ -1758,7 +1698,7 @@
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>0.42708333333333398</v>
       </c>
@@ -1776,17 +1716,6 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="1"/>
-      <c r="N12" s="11" t="s">
-        <v>140</v>
-      </c>
       <c r="O12" s="6">
         <v>0.42708333333333398</v>
       </c>
@@ -1810,11 +1739,11 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="10" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="10" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
@@ -1822,17 +1751,6 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="L13" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="M13" s="1"/>
-      <c r="N13" s="9" t="s">
-        <v>62</v>
-      </c>
       <c r="O13" s="6">
         <v>0.43055555555555602</v>
       </c>
@@ -1856,11 +1774,11 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="11" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="11" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1868,17 +1786,6 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="K14" s="1"/>
-      <c r="L14" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="M14" s="1"/>
-      <c r="N14" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="O14" s="6">
         <v>0.43402777777777801</v>
       </c>
@@ -1914,15 +1821,13 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M15" s="1"/>
-      <c r="N15" s="10" t="s">
+      <c r="J15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="O15" s="6">
@@ -1960,15 +1865,13 @@
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" s="1"/>
-      <c r="N16" s="10" t="s">
+      <c r="J16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="O16" s="6">
@@ -1994,28 +1897,28 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="9" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="9" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="9" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="9" t="s">
-        <v>132</v>
+      <c r="J17" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K17" s="1"/>
-      <c r="L17" s="9" t="s">
-        <v>131</v>
+      <c r="L17" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M17" s="1"/>
-      <c r="N17" s="10" t="s">
-        <v>10</v>
+      <c r="N17" s="9" t="s">
+        <v>137</v>
       </c>
       <c r="O17" s="6">
         <v>0.44444444444444497</v>
@@ -2034,7 +1937,7 @@
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>0.44791666666666702</v>
       </c>
@@ -2052,11 +1955,11 @@
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K18" s="1"/>
-      <c r="L18" s="10" t="s">
+      <c r="L18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M18" s="1"/>
@@ -2098,16 +2001,16 @@
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="10" t="s">
-        <v>10</v>
+      <c r="J19" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="K19" s="1"/>
-      <c r="L19" s="10" t="s">
-        <v>10</v>
+      <c r="L19" s="9" t="s">
+        <v>132</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="10" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="O19" s="6">
         <v>0.45138888888889001</v>
@@ -2126,7 +2029,7 @@
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
     </row>
-    <row r="20" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>0.45486111111111199</v>
       </c>
@@ -2152,8 +2055,8 @@
         <v>10</v>
       </c>
       <c r="M20" s="1"/>
-      <c r="N20" s="11" t="s">
-        <v>130</v>
+      <c r="N20" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="O20" s="6">
         <v>0.45486111111111199</v>
@@ -2198,8 +2101,8 @@
         <v>10</v>
       </c>
       <c r="M21" s="1"/>
-      <c r="N21" s="9" t="s">
-        <v>129</v>
+      <c r="N21" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="O21" s="6">
         <v>0.45833333333333398</v>
@@ -2270,11 +2173,11 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="10" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="10" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="10" t="s">
@@ -2283,15 +2186,15 @@
       <c r="H23" s="18"/>
       <c r="I23" s="1"/>
       <c r="J23" s="10" t="s">
-        <v>126</v>
+        <v>10</v>
       </c>
       <c r="K23" s="1"/>
       <c r="L23" s="10" t="s">
-        <v>125</v>
+        <v>10</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="10" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="O23" s="6">
         <v>0.46527777777777901</v>
@@ -2316,11 +2219,11 @@
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="11" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="11" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="10" t="s">
@@ -2328,16 +2231,16 @@
       </c>
       <c r="H24" s="18"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="11" t="s">
-        <v>124</v>
+      <c r="J24" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="K24" s="1"/>
-      <c r="L24" s="11" t="s">
-        <v>124</v>
+      <c r="L24" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="M24" s="1"/>
-      <c r="N24" s="10" t="s">
-        <v>10</v>
+      <c r="N24" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="O24" s="6">
         <v>0.468750000000001</v>
@@ -2374,16 +2277,16 @@
       </c>
       <c r="H25" s="18"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1" t="s">
-        <v>10</v>
+      <c r="J25" s="10" t="s">
+        <v>129</v>
       </c>
       <c r="K25" s="1"/>
-      <c r="L25" s="1" t="s">
-        <v>10</v>
+      <c r="L25" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="M25" s="1"/>
-      <c r="N25" s="10" t="s">
-        <v>10</v>
+      <c r="N25" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="O25" s="6">
         <v>0.47222222222222299</v>
@@ -2420,12 +2323,12 @@
       </c>
       <c r="H26" s="18"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="1" t="s">
-        <v>10</v>
+      <c r="J26" s="11" t="s">
+        <v>203</v>
       </c>
       <c r="K26" s="1"/>
-      <c r="L26" s="1" t="s">
-        <v>10</v>
+      <c r="L26" s="11" t="s">
+        <v>203</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="10" t="s">
@@ -2454,24 +2357,24 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="9" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="10" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="9" t="s">
-        <v>120</v>
+      <c r="J27" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K27" s="1"/>
-      <c r="L27" s="9" t="s">
-        <v>119</v>
+      <c r="L27" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M27" s="1"/>
       <c r="N27" s="10" t="s">
@@ -2508,15 +2411,15 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="11" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H28" s="18"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="10" t="s">
+      <c r="J28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K28" s="1"/>
-      <c r="L28" s="10" t="s">
+      <c r="L28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M28" s="1"/>
@@ -2558,12 +2461,12 @@
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="10" t="s">
-        <v>10</v>
+      <c r="J29" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="K29" s="1"/>
-      <c r="L29" s="10" t="s">
-        <v>10</v>
+      <c r="L29" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="M29" s="1"/>
       <c r="N29" s="10" t="s">
@@ -2646,7 +2549,7 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="9" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="1"/>
@@ -2659,7 +2562,7 @@
       </c>
       <c r="M31" s="1"/>
       <c r="N31" s="10" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="O31" s="6">
         <v>0.49305555555555702</v>
@@ -2705,7 +2608,7 @@
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="11" t="s">
-        <v>115</v>
+        <v>212</v>
       </c>
       <c r="O32" s="6">
         <v>0.49652777777777901</v>
@@ -2730,11 +2633,11 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
@@ -2743,15 +2646,15 @@
       <c r="H33" s="18"/>
       <c r="I33" s="1"/>
       <c r="J33" s="10" t="s">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="10" t="s">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="M33" s="1"/>
       <c r="N33" s="9" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="O33" s="6">
         <v>0.500000000000001</v>
@@ -2776,11 +2679,11 @@
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="11" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="11" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="10" t="s">
@@ -2788,12 +2691,12 @@
       </c>
       <c r="H34" s="18"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="11" t="s">
-        <v>109</v>
+      <c r="J34" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="K34" s="1"/>
-      <c r="L34" s="11" t="s">
-        <v>109</v>
+      <c r="L34" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="M34" s="1"/>
       <c r="N34" s="10" t="s">
@@ -2834,12 +2737,12 @@
       </c>
       <c r="H35" s="18"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="1" t="s">
-        <v>10</v>
+      <c r="J35" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="K35" s="1"/>
-      <c r="L35" s="1" t="s">
-        <v>10</v>
+      <c r="L35" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="M35" s="1"/>
       <c r="N35" s="10" t="s">
@@ -2880,12 +2783,12 @@
       </c>
       <c r="H36" s="18"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="1" t="s">
-        <v>10</v>
+      <c r="J36" s="11" t="s">
+        <v>204</v>
       </c>
       <c r="K36" s="1"/>
-      <c r="L36" s="1" t="s">
-        <v>10</v>
+      <c r="L36" s="11" t="s">
+        <v>204</v>
       </c>
       <c r="M36" s="1"/>
       <c r="N36" s="10" t="s">
@@ -2914,11 +2817,11 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="9" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="9" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="10" t="s">
@@ -2954,7 +2857,7 @@
       <c r="AA37" s="1"/>
       <c r="AB37" s="1"/>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
         <v>0.51736111111111205</v>
       </c>
@@ -3010,7 +2913,7 @@
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="10" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="10" t="s">
@@ -3018,12 +2921,12 @@
       </c>
       <c r="H39" s="18"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="1" t="s">
-        <v>10</v>
+      <c r="J39" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="K39" s="1"/>
-      <c r="L39" s="1" t="s">
-        <v>10</v>
+      <c r="L39" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="M39" s="1"/>
       <c r="N39" s="10" t="s">
@@ -3056,7 +2959,7 @@
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="11" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="10" t="s">
@@ -3064,11 +2967,11 @@
       </c>
       <c r="H40" s="18"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="1" t="s">
+      <c r="J40" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K40" s="1"/>
-      <c r="L40" s="1" t="s">
+      <c r="L40" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M40" s="1"/>
@@ -3106,15 +3009,15 @@
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="10" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="H41" s="18"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="1" t="s">
+      <c r="J41" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K41" s="1"/>
-      <c r="L41" s="1" t="s">
+      <c r="L41" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M41" s="1"/>
@@ -3152,15 +3055,15 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="11" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H42" s="18"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="1" t="s">
+      <c r="J42" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K42" s="1"/>
-      <c r="L42" s="1" t="s">
+      <c r="L42" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M42" s="1"/>
@@ -3190,7 +3093,7 @@
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="10" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
@@ -3202,16 +3105,16 @@
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="1" t="s">
+      <c r="J43" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K43" s="1"/>
-      <c r="L43" s="1" t="s">
+      <c r="L43" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M43" s="1"/>
       <c r="N43" s="10" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="O43" s="6">
         <v>0.53472222222222399</v>
@@ -3236,7 +3139,7 @@
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
@@ -3248,16 +3151,16 @@
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="1" t="s">
+      <c r="J44" s="10" t="s">
         <v>10</v>
       </c>
       <c r="K44" s="1"/>
-      <c r="L44" s="1" t="s">
+      <c r="L44" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M44" s="1"/>
       <c r="N44" s="11" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="O44" s="6">
         <v>0.53819444444444597</v>
@@ -3294,16 +3197,16 @@
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="9" t="s">
-        <v>99</v>
+      <c r="J45" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="K45" s="1"/>
-      <c r="L45" s="9" t="s">
-        <v>98</v>
+      <c r="L45" s="10" t="s">
+        <v>104</v>
       </c>
       <c r="M45" s="1"/>
       <c r="N45" s="9" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="O45" s="6">
         <v>0.54166666666666796</v>
@@ -3322,7 +3225,7 @@
       <c r="AA45" s="1"/>
       <c r="AB45" s="1"/>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
         <v>0.54513888888888995</v>
       </c>
@@ -3340,12 +3243,12 @@
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="10" t="s">
-        <v>10</v>
+      <c r="J46" s="11" t="s">
+        <v>205</v>
       </c>
       <c r="K46" s="1"/>
-      <c r="L46" s="10" t="s">
-        <v>10</v>
+      <c r="L46" s="11" t="s">
+        <v>205</v>
       </c>
       <c r="M46" s="1"/>
       <c r="N46" s="10" t="s">
@@ -3386,11 +3289,11 @@
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="J47" s="10" t="s">
+      <c r="J47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K47" s="1"/>
-      <c r="L47" s="10" t="s">
+      <c r="L47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M47" s="1"/>
@@ -3432,11 +3335,11 @@
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="10" t="s">
+      <c r="J48" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K48" s="1"/>
-      <c r="L48" s="10" t="s">
+      <c r="L48" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M48" s="1"/>
@@ -3478,11 +3381,11 @@
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="J49" s="10" t="s">
+      <c r="J49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K49" s="1"/>
-      <c r="L49" s="10" t="s">
+      <c r="L49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M49" s="1"/>
@@ -3524,11 +3427,11 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="10" t="s">
+      <c r="J50" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K50" s="1"/>
-      <c r="L50" s="10" t="s">
+      <c r="L50" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M50" s="1"/>
@@ -3562,7 +3465,7 @@
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="9" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
@@ -3570,12 +3473,12 @@
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-      <c r="J51" s="10" t="s">
-        <v>95</v>
+      <c r="J51" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K51" s="1"/>
-      <c r="L51" s="10" t="s">
-        <v>94</v>
+      <c r="L51" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M51" s="1"/>
       <c r="N51" s="10" t="s">
@@ -3616,12 +3519,12 @@
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="11" t="s">
-        <v>93</v>
+      <c r="J52" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K52" s="1"/>
-      <c r="L52" s="11" t="s">
-        <v>93</v>
+      <c r="L52" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M52" s="1"/>
       <c r="N52" s="10" t="s">
@@ -3658,7 +3561,7 @@
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="1"/>
@@ -3742,7 +3645,7 @@
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="9" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="10" t="s">
@@ -3754,16 +3657,16 @@
       </c>
       <c r="H55" s="18"/>
       <c r="I55" s="1"/>
-      <c r="J55" s="9" t="s">
-        <v>90</v>
+      <c r="J55" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K55" s="1"/>
-      <c r="L55" s="9" t="s">
-        <v>89</v>
+      <c r="L55" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M55" s="1"/>
       <c r="N55" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="O55" s="6">
         <v>0.57638888888889095</v>
@@ -3800,16 +3703,16 @@
       </c>
       <c r="H56" s="18"/>
       <c r="I56" s="1"/>
-      <c r="J56" s="10" t="s">
+      <c r="J56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K56" s="1"/>
-      <c r="L56" s="10" t="s">
+      <c r="L56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M56" s="1"/>
       <c r="N56" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="O56" s="6">
         <v>0.57986111111111305</v>
@@ -3834,11 +3737,11 @@
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="10" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="10" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="10" t="s">
@@ -3846,16 +3749,16 @@
       </c>
       <c r="H57" s="18"/>
       <c r="I57" s="1"/>
-      <c r="J57" s="10" t="s">
-        <v>10</v>
+      <c r="J57" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="K57" s="1"/>
-      <c r="L57" s="10" t="s">
-        <v>10</v>
+      <c r="L57" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="M57" s="1"/>
       <c r="N57" s="9" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="O57" s="6">
         <v>0.58333333333333504</v>
@@ -3880,11 +3783,11 @@
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="11" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="10" t="s">
@@ -4018,11 +3921,11 @@
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="10" t="s">
@@ -4031,11 +3934,11 @@
       <c r="H61" s="18"/>
       <c r="I61" s="1"/>
       <c r="J61" s="10" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="K61" s="1"/>
       <c r="L61" s="10" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="M61" s="1"/>
       <c r="N61" s="10" t="s">
@@ -4058,7 +3961,7 @@
       <c r="AA61" s="1"/>
       <c r="AB61" s="1"/>
     </row>
-    <row r="62" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>0.60069444444444697</v>
       </c>
@@ -4076,12 +3979,12 @@
       </c>
       <c r="H62" s="18"/>
       <c r="I62" s="1"/>
-      <c r="J62" s="11" t="s">
-        <v>77</v>
+      <c r="J62" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="K62" s="1"/>
-      <c r="L62" s="11" t="s">
-        <v>77</v>
+      <c r="L62" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="M62" s="1"/>
       <c r="N62" s="10" t="s">
@@ -4110,24 +4013,24 @@
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H63" s="18"/>
       <c r="I63" s="1"/>
-      <c r="J63" s="1" t="s">
-        <v>10</v>
+      <c r="J63" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="K63" s="1"/>
-      <c r="L63" s="1" t="s">
-        <v>10</v>
+      <c r="L63" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="M63" s="1"/>
       <c r="N63" s="10" t="s">
@@ -4156,24 +4059,24 @@
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H64" s="18"/>
       <c r="I64" s="1"/>
-      <c r="J64" s="1" t="s">
-        <v>10</v>
+      <c r="J64" s="11" t="s">
+        <v>206</v>
       </c>
       <c r="K64" s="1"/>
-      <c r="L64" s="1" t="s">
-        <v>10</v>
+      <c r="L64" s="11" t="s">
+        <v>206</v>
       </c>
       <c r="M64" s="1"/>
       <c r="N64" s="10" t="s">
@@ -4214,12 +4117,12 @@
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
-      <c r="J65" s="9" t="s">
-        <v>71</v>
+      <c r="J65" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K65" s="1"/>
-      <c r="L65" s="9" t="s">
-        <v>70</v>
+      <c r="L65" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M65" s="1"/>
       <c r="N65" s="10" t="s">
@@ -4260,11 +4163,11 @@
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
-      <c r="J66" s="10" t="s">
+      <c r="J66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K66" s="1"/>
-      <c r="L66" s="10" t="s">
+      <c r="L66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M66" s="1"/>
@@ -4294,28 +4197,28 @@
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="9" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H67" s="17"/>
       <c r="I67" s="1"/>
-      <c r="J67" s="10" t="s">
-        <v>10</v>
+      <c r="J67" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="K67" s="1"/>
-      <c r="L67" s="10" t="s">
-        <v>10</v>
+      <c r="L67" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="M67" s="1"/>
       <c r="N67" s="10" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="O67" s="6">
         <v>0.61805555555555802</v>
@@ -4361,7 +4264,7 @@
       </c>
       <c r="M68" s="1"/>
       <c r="N68" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="O68" s="6">
         <v>0.62152777777778001</v>
@@ -4386,11 +4289,11 @@
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="10" t="s">
@@ -4407,7 +4310,7 @@
       </c>
       <c r="M69" s="1"/>
       <c r="N69" s="9" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="O69" s="6">
         <v>0.625000000000003</v>
@@ -4432,11 +4335,11 @@
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="10" t="s">
@@ -4491,11 +4394,11 @@
       <c r="H71" s="18"/>
       <c r="I71" s="1"/>
       <c r="J71" s="10" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="K71" s="1"/>
       <c r="L71" s="10" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="M71" s="1"/>
       <c r="N71" s="10" t="s">
@@ -4536,12 +4439,12 @@
       </c>
       <c r="H72" s="18"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="11" t="s">
-        <v>58</v>
+      <c r="J72" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="K72" s="1"/>
-      <c r="L72" s="11" t="s">
-        <v>58</v>
+      <c r="L72" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="M72" s="1"/>
       <c r="N72" s="10" t="s">
@@ -4570,11 +4473,11 @@
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="10" t="s">
@@ -4582,12 +4485,12 @@
       </c>
       <c r="H73" s="18"/>
       <c r="I73" s="1"/>
-      <c r="J73" s="1" t="s">
-        <v>10</v>
+      <c r="J73" s="10" t="s">
+        <v>207</v>
       </c>
       <c r="K73" s="1"/>
-      <c r="L73" s="1" t="s">
-        <v>10</v>
+      <c r="L73" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="M73" s="1"/>
       <c r="N73" s="10" t="s">
@@ -4628,12 +4531,12 @@
       </c>
       <c r="H74" s="18"/>
       <c r="I74" s="1"/>
-      <c r="J74" s="1" t="s">
-        <v>10</v>
+      <c r="J74" s="11" t="s">
+        <v>208</v>
       </c>
       <c r="K74" s="1"/>
-      <c r="L74" s="1" t="s">
-        <v>10</v>
+      <c r="L74" s="11" t="s">
+        <v>208</v>
       </c>
       <c r="M74" s="1"/>
       <c r="N74" s="10" t="s">
@@ -4662,11 +4565,11 @@
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="10" t="s">
@@ -4674,12 +4577,12 @@
       </c>
       <c r="H75" s="18"/>
       <c r="I75" s="1"/>
-      <c r="J75" s="9" t="s">
-        <v>53</v>
+      <c r="J75" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K75" s="1"/>
-      <c r="L75" s="9" t="s">
-        <v>52</v>
+      <c r="L75" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M75" s="1"/>
       <c r="N75" s="10" t="s">
@@ -4708,11 +4611,11 @@
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="10" t="s">
@@ -4720,11 +4623,11 @@
       </c>
       <c r="H76" s="18"/>
       <c r="I76" s="1"/>
-      <c r="J76" s="10" t="s">
+      <c r="J76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K76" s="1"/>
-      <c r="L76" s="10" t="s">
+      <c r="L76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M76" s="1"/>
@@ -4762,16 +4665,16 @@
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H77" s="18"/>
       <c r="I77" s="1"/>
-      <c r="J77" s="10" t="s">
-        <v>10</v>
+      <c r="J77" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="K77" s="1"/>
-      <c r="L77" s="10" t="s">
-        <v>10</v>
+      <c r="L77" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="M77" s="1"/>
       <c r="N77" s="10" t="s">
@@ -4808,7 +4711,7 @@
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H78" s="18"/>
       <c r="I78" s="1"/>
@@ -4846,11 +4749,11 @@
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F79" s="1"/>
       <c r="G79" s="1" t="s">
@@ -4867,7 +4770,7 @@
       </c>
       <c r="M79" s="1"/>
       <c r="N79" s="10" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="O79" s="6">
         <v>0.65972222222222499</v>
@@ -4913,7 +4816,7 @@
       </c>
       <c r="M80" s="1"/>
       <c r="N80" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="O80" s="6">
         <v>0.66319444444444697</v>
@@ -4946,20 +4849,20 @@
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H81" s="17"/>
       <c r="I81" s="1"/>
       <c r="J81" s="10" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="K81" s="1"/>
       <c r="L81" s="10" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="M81" s="1"/>
       <c r="N81" s="9" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="O81" s="6">
         <v>0.66666666666666996</v>
@@ -4978,7 +4881,7 @@
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
     </row>
-    <row r="82" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>0.67013888888889195</v>
       </c>
@@ -4996,12 +4899,12 @@
       </c>
       <c r="H82" s="18"/>
       <c r="I82" s="1"/>
-      <c r="J82" s="11" t="s">
-        <v>40</v>
+      <c r="J82" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="K82" s="1"/>
-      <c r="L82" s="11" t="s">
-        <v>40</v>
+      <c r="L82" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="M82" s="1"/>
       <c r="N82" s="10" t="s">
@@ -5042,12 +4945,12 @@
       </c>
       <c r="H83" s="18"/>
       <c r="I83" s="1"/>
-      <c r="J83" s="1" t="s">
-        <v>10</v>
+      <c r="J83" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="K83" s="1"/>
-      <c r="L83" s="1" t="s">
-        <v>10</v>
+      <c r="L83" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="M83" s="1"/>
       <c r="N83" s="10" t="s">
@@ -5088,12 +4991,12 @@
       </c>
       <c r="H84" s="18"/>
       <c r="I84" s="1"/>
-      <c r="J84" s="1" t="s">
-        <v>10</v>
+      <c r="J84" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="K84" s="1"/>
-      <c r="L84" s="1" t="s">
-        <v>10</v>
+      <c r="L84" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="M84" s="1"/>
       <c r="N84" s="10" t="s">
@@ -5122,11 +5025,11 @@
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="10" t="s">
@@ -5134,12 +5037,12 @@
       </c>
       <c r="H85" s="18"/>
       <c r="I85" s="1"/>
-      <c r="J85" s="9" t="s">
-        <v>37</v>
+      <c r="J85" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="K85" s="1"/>
-      <c r="L85" s="9" t="s">
-        <v>36</v>
+      <c r="L85" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="M85" s="1"/>
       <c r="N85" s="10" t="s">
@@ -5168,11 +5071,11 @@
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="10" t="s">
@@ -5180,11 +5083,11 @@
       </c>
       <c r="H86" s="18"/>
       <c r="I86" s="1"/>
-      <c r="J86" s="10" t="s">
+      <c r="J86" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K86" s="1"/>
-      <c r="L86" s="10" t="s">
+      <c r="L86" s="1" t="s">
         <v>10</v>
       </c>
       <c r="M86" s="1"/>
@@ -5226,12 +5129,12 @@
       </c>
       <c r="H87" s="18"/>
       <c r="I87" s="1"/>
-      <c r="J87" s="10" t="s">
-        <v>10</v>
+      <c r="J87" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="K87" s="1"/>
-      <c r="L87" s="10" t="s">
-        <v>10</v>
+      <c r="L87" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="M87" s="1"/>
       <c r="N87" s="10" t="s">
@@ -5306,11 +5209,11 @@
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="10" t="s">
@@ -5406,20 +5309,20 @@
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H91" s="18"/>
       <c r="I91" s="1"/>
       <c r="J91" s="10" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="K91" s="1"/>
       <c r="L91" s="10" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="M91" s="1"/>
       <c r="N91" s="10" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="O91" s="6">
         <v>0.70138888888889195</v>
@@ -5452,20 +5355,20 @@
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H92" s="18"/>
       <c r="I92" s="1"/>
-      <c r="J92" s="11" t="s">
-        <v>28</v>
+      <c r="J92" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="K92" s="1"/>
-      <c r="L92" s="11" t="s">
-        <v>28</v>
+      <c r="L92" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="M92" s="1"/>
       <c r="N92" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O92" s="6">
         <v>0.70486111111111505</v>
@@ -5502,15 +5405,17 @@
       </c>
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
-      <c r="J93" s="1" t="s">
-        <v>10</v>
+      <c r="J93" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="K93" s="1"/>
-      <c r="L93" s="1" t="s">
-        <v>10</v>
+      <c r="L93" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="M93" s="1"/>
-      <c r="N93" s="1"/>
+      <c r="N93" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="O93" s="6">
         <v>0.70833333333333703</v>
       </c>
@@ -5546,15 +5451,17 @@
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
-      <c r="J94" s="1" t="s">
-        <v>10</v>
+      <c r="J94" s="11" t="s">
+        <v>210</v>
       </c>
       <c r="K94" s="1"/>
-      <c r="L94" s="1" t="s">
-        <v>10</v>
+      <c r="L94" s="11" t="s">
+        <v>210</v>
       </c>
       <c r="M94" s="1"/>
-      <c r="N94" s="1"/>
+      <c r="N94" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O94" s="6">
         <v>0.71180555555555902</v>
       </c>
@@ -5578,15 +5485,15 @@
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F95" s="1"/>
-      <c r="G95" s="9" t="s">
-        <v>24</v>
+      <c r="G95" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="H95" s="17"/>
       <c r="I95" s="1"/>
@@ -5598,7 +5505,9 @@
         <v>10</v>
       </c>
       <c r="M95" s="1"/>
-      <c r="N95" s="1"/>
+      <c r="N95" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O95" s="6">
         <v>0.71527777777778101</v>
       </c>
@@ -5622,14 +5531,14 @@
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F96" s="1"/>
-      <c r="G96" s="10" t="s">
+      <c r="G96" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H96" s="18"/>
@@ -5642,7 +5551,9 @@
         <v>10</v>
       </c>
       <c r="M96" s="1"/>
-      <c r="N96" s="1"/>
+      <c r="N96" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O96" s="6">
         <v>0.718750000000004</v>
       </c>
@@ -5673,16 +5584,22 @@
         <v>10</v>
       </c>
       <c r="F97" s="1"/>
-      <c r="G97" s="10" t="s">
-        <v>10</v>
+      <c r="G97" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="H97" s="18"/>
       <c r="I97" s="1"/>
-      <c r="J97" s="1"/>
+      <c r="J97" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="K97" s="1"/>
-      <c r="L97" s="1"/>
+      <c r="L97" s="9" t="s">
+        <v>34</v>
+      </c>
       <c r="M97" s="1"/>
-      <c r="N97" s="1"/>
+      <c r="N97" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O97" s="6">
         <v>0.72222222222222598</v>
       </c>
@@ -5718,11 +5635,17 @@
       </c>
       <c r="H98" s="18"/>
       <c r="I98" s="1"/>
-      <c r="J98" s="1"/>
+      <c r="J98" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="K98" s="1"/>
-      <c r="L98" s="1"/>
+      <c r="L98" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="M98" s="1"/>
-      <c r="N98" s="1"/>
+      <c r="N98" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O98" s="6">
         <v>0.72569444444444797</v>
       </c>
@@ -5746,11 +5669,11 @@
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="10" t="s">
@@ -5758,11 +5681,17 @@
       </c>
       <c r="H99" s="18"/>
       <c r="I99" s="1"/>
-      <c r="J99" s="1"/>
+      <c r="J99" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="K99" s="1"/>
-      <c r="L99" s="1"/>
+      <c r="L99" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="M99" s="1"/>
-      <c r="N99" s="1"/>
+      <c r="N99" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O99" s="6">
         <v>0.72916666666666996</v>
       </c>
@@ -5798,11 +5727,17 @@
       </c>
       <c r="H100" s="18"/>
       <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
+      <c r="J100" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="K100" s="1"/>
-      <c r="L100" s="1"/>
+      <c r="L100" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="M100" s="1"/>
-      <c r="N100" s="1"/>
+      <c r="N100" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O100" s="6">
         <v>0.73263888888889295</v>
       </c>
@@ -5826,11 +5761,11 @@
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="10" t="s">
@@ -5838,11 +5773,17 @@
       </c>
       <c r="H101" s="18"/>
       <c r="I101" s="1"/>
-      <c r="J101" s="1"/>
+      <c r="J101" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="K101" s="1"/>
-      <c r="L101" s="1"/>
+      <c r="L101" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
+      <c r="N101" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O101" s="6">
         <v>0.73611111111111505</v>
       </c>
@@ -5865,11 +5806,11 @@
         <v>0.73958333333333703</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="10" t="s">
@@ -5877,11 +5818,17 @@
       </c>
       <c r="H102" s="18"/>
       <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
+      <c r="J102" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="K102" s="1"/>
-      <c r="L102" s="1"/>
+      <c r="L102" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
+      <c r="N102" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="O102" s="6">
         <v>0.73958333333333703</v>
       </c>
@@ -5905,11 +5852,17 @@
       </c>
       <c r="H103" s="18"/>
       <c r="I103" s="1"/>
-      <c r="J103" s="1"/>
+      <c r="J103" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="K103" s="1"/>
-      <c r="L103" s="1"/>
+      <c r="L103" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="M103" s="1"/>
-      <c r="N103" s="1"/>
+      <c r="N103" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="O103" s="6">
         <v>0.74305555555556002</v>
       </c>
@@ -5933,11 +5886,17 @@
       </c>
       <c r="H104" s="18"/>
       <c r="I104" s="1"/>
-      <c r="J104" s="1"/>
+      <c r="J104" s="11" t="s">
+        <v>211</v>
+      </c>
       <c r="K104" s="1"/>
-      <c r="L104" s="1"/>
+      <c r="L104" s="11" t="s">
+        <v>211</v>
+      </c>
       <c r="M104" s="1"/>
-      <c r="N104" s="1"/>
+      <c r="N104" s="11" t="s">
+        <v>213</v>
+      </c>
       <c r="O104" s="6">
         <v>0.74652777777778201</v>
       </c>
@@ -5949,21 +5908,25 @@
         <v>0.750000000000004</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H105" s="18"/>
       <c r="I105" s="1"/>
-      <c r="J105" s="1"/>
+      <c r="J105" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K105" s="1"/>
-      <c r="L105" s="1"/>
+      <c r="L105" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
       <c r="O105" s="6">
@@ -5972,7 +5935,7 @@
       <c r="P105" s="1"/>
       <c r="Q105" s="1"/>
     </row>
-    <row r="106" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A106" s="6">
         <v>0.75347222222222598</v>
       </c>
@@ -5984,14 +5947,18 @@
         <v>10</v>
       </c>
       <c r="F106" s="1"/>
-      <c r="G106" s="11" t="s">
-        <v>14</v>
+      <c r="G106" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="H106" s="18"/>
       <c r="I106" s="1"/>
-      <c r="J106" s="1"/>
+      <c r="J106" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K106" s="1"/>
-      <c r="L106" s="1"/>
+      <c r="L106" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
       <c r="O106" s="6">
@@ -6012,12 +5979,18 @@
         <v>12</v>
       </c>
       <c r="F107" s="1"/>
-      <c r="G107" s="1"/>
+      <c r="G107" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
-      <c r="J107" s="1"/>
+      <c r="J107" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K107" s="1"/>
-      <c r="L107" s="1"/>
+      <c r="L107" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
       <c r="O107" s="6">
@@ -6038,12 +6011,18 @@
         <v>11</v>
       </c>
       <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
+      <c r="G108" s="11" t="s">
+        <v>200</v>
+      </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
-      <c r="J108" s="1"/>
+      <c r="J108" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K108" s="1"/>
-      <c r="L108" s="1"/>
+      <c r="L108" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
       <c r="O108" s="6">
@@ -6154,11 +6133,18 @@
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="6"/>
-      <c r="O113" s="6"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A114" s="6"/>
-      <c r="O114" s="6"/>
+      <c r="A114" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="B114" s="22"/>
+      <c r="C114" s="23"/>
+      <c r="N114" s="19" t="str">
+        <f>A114</f>
+        <v>Last updated: 27.06.2017 14:55</v>
+      </c>
+      <c r="O114" s="20"/>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" s="6"/>
@@ -6273,8 +6259,12 @@
       <c r="O142" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="N114:O114"/>
+    <mergeCell ref="A114:C114"/>
+  </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="44" fitToWidth="2" orientation="portrait" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="43" fitToWidth="2" orientation="portrait" blackAndWhite="1" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="44" max="16383" man="1"/>
   </rowBreaks>
@@ -6291,8 +6281,8 @@
   </sheetPr>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A29" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6308,25 +6298,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -6337,13 +6327,13 @@
         <v>0.40972222222222227</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -6356,41 +6346,41 @@
         <v>0.40972222222222227</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>0.40277777777777773</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="B4" s="14">
-        <v>0.43055555555555558</v>
+        <v>0.4375</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>157</v>
+        <v>201</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>0.40972222222222227</v>
       </c>
@@ -6398,1123 +6388,1123 @@
         <v>0.4375</v>
       </c>
       <c r="C5" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="B7" s="14">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
-        <v>0.40972222222222227</v>
-      </c>
-      <c r="B6" s="14">
-        <v>0.4375</v>
-      </c>
-      <c r="C6" s="15" t="s">
+      <c r="D8" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
-        <v>0.40972222222222227</v>
-      </c>
-      <c r="B7" s="14">
-        <v>0.4375</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>0.40972222222222227</v>
-      </c>
-      <c r="B8" s="14">
-        <v>0.4375</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>162</v>
-      </c>
       <c r="G8" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
-        <v>0.43055555555555558</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="B9" s="14">
-        <v>0.45833333333333331</v>
+        <v>0.47222222222222227</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>46</v>
+        <v>131</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
-        <v>0.44444444444444442</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="B10" s="14">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
         <v>0.47222222222222227</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="B11" s="14">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="210" x14ac:dyDescent="0.25">
-      <c r="A12" s="14">
-        <v>0.44444444444444442</v>
-      </c>
       <c r="B12" s="14">
-        <v>0.4861111111111111</v>
+        <v>0.5</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>167</v>
+        <v>7</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>121</v>
+        <v>43</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>133</v>
+        <v>58</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
-        <v>0.44444444444444442</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="B13" s="14">
-        <v>0.47222222222222227</v>
+        <v>0.50694444444444442</v>
       </c>
       <c r="C13" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="B14" s="14">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="B15" s="14">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="G13" s="15" t="s">
+      <c r="D15" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="B14" s="14">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="C14" s="15" t="s">
+      <c r="G15" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="B16" s="14">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="B15" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="B16" s="14">
-        <v>0.50694444444444442</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>155</v>
-      </c>
       <c r="D16" s="15" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
-        <v>0.47916666666666669</v>
+        <v>0.49305555555555558</v>
       </c>
       <c r="B17" s="14">
-        <v>0.50694444444444442</v>
+        <v>0.53472222222222221</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="G17" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="B18" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="B19" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="B20" s="14">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B21" s="14">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="B22" s="14">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B23" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="15" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="B18" s="14">
-        <v>0.50694444444444442</v>
-      </c>
-      <c r="C18" s="15" t="s">
+      <c r="G23" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="14">
+        <v>0.5625</v>
+      </c>
+      <c r="B24" s="14">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="14">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="B25" s="14">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="B26" s="14">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B27" s="14">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="B19" s="14">
-        <v>0.50694444444444442</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
-        <v>0.49305555555555558</v>
-      </c>
-      <c r="B20" s="14">
-        <v>0.53472222222222221</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="B21" s="14">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="15" t="s">
+      <c r="D27" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="G21" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="B22" s="14">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="B23" s="14">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="G23" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="B24" s="14">
-        <v>0.56944444444444442</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="B25" s="14">
-        <v>0.56944444444444442</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="B26" s="14">
+      <c r="E27" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
         <v>0.58333333333333337</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" s="14">
-        <v>0.5625</v>
-      </c>
-      <c r="B27" s="14">
-        <v>0.59027777777777779</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="14">
-        <v>0.56944444444444442</v>
       </c>
       <c r="B28" s="14">
         <v>0.61111111111111105</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>167</v>
+        <v>6</v>
       </c>
       <c r="D28" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B29" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="B30" s="14">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="B31" s="14">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
-        <v>0.57638888888888895</v>
-      </c>
-      <c r="B29" s="14">
-        <v>0.59027777777777779</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
-        <v>0.57638888888888895</v>
-      </c>
-      <c r="B30" s="14">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
-        <v>0.57638888888888895</v>
-      </c>
-      <c r="B31" s="14">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>89</v>
-      </c>
       <c r="F31" s="15" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
-        <v>0.58333333333333337</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="B32" s="14">
-        <v>0.625</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
-        <v>0.59722222222222221</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="B33" s="14">
-        <v>0.61111111111111105</v>
+        <v>0.63194444444444442</v>
       </c>
       <c r="C33" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="B34" s="14">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="D33" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
-        <v>0.59722222222222221</v>
-      </c>
-      <c r="B34" s="14">
-        <v>0.61111111111111105</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>156</v>
-      </c>
       <c r="D34" s="15" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
-        <v>0.61111111111111105</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="B35" s="14">
-        <v>0.63888888888888895</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>60</v>
+        <v>207</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
-        <v>0.61111111111111105</v>
+        <v>0.61805555555555558</v>
       </c>
       <c r="B36" s="14">
-        <v>0.63888888888888895</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
-        <v>0.61805555555555558</v>
+        <v>0.625</v>
       </c>
       <c r="B37" s="14">
-        <v>0.63194444444444442</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>155</v>
+        <v>7</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
-        <v>0.61805555555555558</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="B38" s="14">
-        <v>0.63194444444444442</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
-        <v>0.61805555555555558</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="B39" s="14">
-        <v>0.65972222222222221</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E39" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="B40" s="14">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
-        <v>0.625</v>
-      </c>
-      <c r="B40" s="14">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E40" s="15" t="s">
-        <v>62</v>
-      </c>
       <c r="F40" s="15" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
-        <v>0.63888888888888895</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="B41" s="14">
-        <v>0.65277777777777779</v>
+        <v>0.68055555555555547</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>155</v>
+        <v>6</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>55</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
-        <v>0.63888888888888895</v>
+        <v>0.65972222222222221</v>
       </c>
       <c r="B42" s="14">
-        <v>0.65277777777777779</v>
+        <v>0.6875</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="14">
-        <v>0.64583333333333337</v>
+        <v>0.65972222222222221</v>
       </c>
       <c r="B43" s="14">
-        <v>0.67361111111111116</v>
+        <v>0.6875</v>
       </c>
       <c r="C43" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="14">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B44" s="14">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="G44" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B45" s="14">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="14">
+        <v>0.6875</v>
+      </c>
+      <c r="B46" s="14">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="C46" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="G43" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" s="14">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="B44" s="14">
-        <v>0.67361111111111116</v>
-      </c>
-      <c r="C44" s="15" t="s">
+      <c r="D46" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="G46" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="14">
+        <v>0.6875</v>
+      </c>
+      <c r="B47" s="14">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="C47" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="14">
-        <v>0.65972222222222221</v>
-      </c>
-      <c r="B45" s="14">
-        <v>0.6875</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D45" s="15" t="s">
+      <c r="D47" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E45" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F45" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="G45" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="14">
-        <v>0.65972222222222221</v>
-      </c>
-      <c r="B46" s="14">
-        <v>0.6875</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D46" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E46" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F46" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="G46" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="14">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="B47" s="14">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>32</v>
-      </c>
       <c r="E47" s="15" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
-        <v>0.66666666666666663</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="B48" s="14">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="14">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="B49" s="14">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="14">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="B50" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="C50" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>204</v>
-      </c>
-      <c r="G48" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A49" s="14">
-        <v>0.68055555555555547</v>
-      </c>
-      <c r="B49" s="14">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="G49" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="14">
-        <v>0.68055555555555547</v>
-      </c>
-      <c r="B50" s="14">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>6</v>
-      </c>
       <c r="D50" s="15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="14">
-        <v>0.69444444444444453</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="B51" s="14">
-        <v>0.72222222222222221</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="C51" s="15" t="s">
         <v>155</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E51" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A52" s="14">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="B52" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A53" s="14">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="B53" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="F51" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" s="14">
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="B52" s="14">
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="G52" s="15" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="14">
-        <v>0.71527777777777779</v>
-      </c>
-      <c r="B53" s="14">
-        <v>0.75694444444444453</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>24</v>
-      </c>
       <c r="F53" s="15" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7525,19 +7515,19 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7548,19 +7538,19 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7571,19 +7561,19 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D56" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7594,37 +7584,34 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D57" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="14">
+      <c r="A58">
         <v>0.77083333333333337</v>
       </c>
-      <c r="B58" s="14">
+      <c r="B58">
         <v>0.77777777777777779</v>
       </c>
-      <c r="C58" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15" t="s">
+      <c r="C58" t="s">
+        <v>145</v>
+      </c>
+      <c r="E58" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
UI5Con Agenda Update 28.6.2017 16:20 and Twitter Timeline
</commit_message>
<xml_diff>
--- a/ui5con/downloads/ui5con_2017_agenda.xlsx
+++ b/ui5con/downloads/ui5con_2017_agenda.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="217">
   <si>
     <r>
       <rPr>
@@ -228,15 +228,9 @@
     <t>Aparna Narayanaswamy</t>
   </si>
   <si>
-    <t>Gregor Brett</t>
-  </si>
-  <si>
     <t>Controlling UI5 Apps and FLP via Speech</t>
   </si>
   <si>
-    <t>Building a companion conversational UI for a Fiori App</t>
-  </si>
-  <si>
     <t>Vered Constantin</t>
   </si>
   <si>
@@ -621,9 +615,6 @@
     <t>Session Description: In this session I will discuss options how UI5 web apps can be used as a basis for apps beyond your typical office requirements. While SAP Fiori apps and Fiori LaunchPad are the basis for SAPs Digital Workplace of the future, there exist much more possibilities how the web can be the basis for your digitalization efforts. We are looking into WebAPIs, standards such as WebRTC and 3rd party extensions and how this can be applied in enterprise settings. Adding Cloud APIs into the mix, lots of demand for feature-rich apps can already be fulfilled leveraging the web.</t>
   </si>
   <si>
-    <t>Building a Conversational UI for the Fiori My Inbox app using API.AI. I will run through the code needed and do a live demo.</t>
-  </si>
-  <si>
     <t>Modern browsers provide Web Speech API, enabling the application of speech recognition in web applications.We have developed an application that demonstrates how this browser capability can be leveraged in the FLP as a control mechanism.</t>
   </si>
   <si>
@@ -723,10 +714,13 @@
     <t>In this session, we will demonstrate how to get started on cloud foundry. We will see how to onboard onto the platform, install the necessary tools and deploy a UI5 application which makes use of platform services to persist its data.Prerequisites:Please have Node.js installed on your laptop and your own hanatrial account ready.</t>
   </si>
   <si>
-    <t xml:space="preserve">Let's build a simple FLP plugin (based on a UI5 Component) together. Once deployed to a FLP on Cloud Platform we will start to use the renderer extension api of FLP to place SAPUI5 controls into the FLP UI to improve the user experience of the Lauchpad AND learn that SAPUI5 and Fiori Launchpad are actually of the same kind. Prerequisites:   - Laptop  - an SAP CP trial account </t>
-  </si>
-  <si>
-    <t>Last updated: 27.06.2017 14:55</t>
+    <t>17:30 - 18:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let's build a simple FLP plugin (based on a UI5 Component) together. Once deployed to a FLP on Cloud Platform we will start to use the renderer extension api of FLP to place SAPUI5 controls into the FLP UI to improve the user experience of the Lauchpad AND learn that SAPUI5 and Fiori Launchpad are actually of the same kind. Prerequisites:   Laptop  an SAP CP trial account </t>
+  </si>
+  <si>
+    <t>Last updated: 28.06.2017 16:20</t>
   </si>
 </sst>
 </file>
@@ -1284,9 +1278,7 @@
   </sheetPr>
   <dimension ref="A1:AB142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114:C114"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="50" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1379,11 +1371,11 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
@@ -1494,11 +1486,11 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
@@ -1529,11 +1521,11 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
@@ -1739,11 +1731,11 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
@@ -1774,11 +1766,11 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
@@ -1897,15 +1889,15 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="1"/>
@@ -1918,7 +1910,7 @@
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="O17" s="6">
         <v>0.44444444444444497</v>
@@ -2002,11 +1994,11 @@
       <c r="H19" s="18"/>
       <c r="I19" s="1"/>
       <c r="J19" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K19" s="1"/>
       <c r="L19" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="10" t="s">
@@ -2173,11 +2165,11 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="10" t="s">
@@ -2194,7 +2186,7 @@
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="O23" s="6">
         <v>0.46527777777777901</v>
@@ -2219,11 +2211,11 @@
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="10" t="s">
@@ -2240,7 +2232,7 @@
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O24" s="6">
         <v>0.468750000000001</v>
@@ -2278,15 +2270,15 @@
       <c r="H25" s="18"/>
       <c r="I25" s="1"/>
       <c r="J25" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O25" s="6">
         <v>0.47222222222222299</v>
@@ -2324,11 +2316,11 @@
       <c r="H26" s="18"/>
       <c r="I26" s="1"/>
       <c r="J26" s="11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="10" t="s">
@@ -2357,15 +2349,15 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="1"/>
@@ -2411,7 +2403,7 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H28" s="18"/>
       <c r="I28" s="1"/>
@@ -2462,11 +2454,11 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M29" s="1"/>
       <c r="N29" s="10" t="s">
@@ -2549,7 +2541,7 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="1"/>
@@ -2608,7 +2600,7 @@
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="11" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="O32" s="6">
         <v>0.49652777777777901</v>
@@ -2633,11 +2625,11 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="10" t="s">
@@ -2654,7 +2646,7 @@
       </c>
       <c r="M33" s="1"/>
       <c r="N33" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O33" s="6">
         <v>0.500000000000001</v>
@@ -2679,11 +2671,11 @@
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="10" t="s">
@@ -2738,11 +2730,11 @@
       <c r="H35" s="18"/>
       <c r="I35" s="1"/>
       <c r="J35" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M35" s="1"/>
       <c r="N35" s="10" t="s">
@@ -2784,11 +2776,11 @@
       <c r="H36" s="18"/>
       <c r="I36" s="1"/>
       <c r="J36" s="11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K36" s="1"/>
       <c r="L36" s="11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="M36" s="1"/>
       <c r="N36" s="10" t="s">
@@ -2817,11 +2809,11 @@
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="10" t="s">
@@ -2913,7 +2905,7 @@
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="10" t="s">
@@ -2922,11 +2914,11 @@
       <c r="H39" s="18"/>
       <c r="I39" s="1"/>
       <c r="J39" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K39" s="1"/>
       <c r="L39" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M39" s="1"/>
       <c r="N39" s="10" t="s">
@@ -2959,7 +2951,7 @@
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="10" t="s">
@@ -3009,7 +3001,7 @@
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H41" s="18"/>
       <c r="I41" s="1"/>
@@ -3055,7 +3047,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H42" s="18"/>
       <c r="I42" s="1"/>
@@ -3093,7 +3085,7 @@
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
@@ -3114,7 +3106,7 @@
       </c>
       <c r="M43" s="1"/>
       <c r="N43" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O43" s="6">
         <v>0.53472222222222399</v>
@@ -3139,7 +3131,7 @@
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
@@ -3160,7 +3152,7 @@
       </c>
       <c r="M44" s="1"/>
       <c r="N44" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O44" s="6">
         <v>0.53819444444444597</v>
@@ -3198,15 +3190,15 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K45" s="1"/>
       <c r="L45" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M45" s="1"/>
       <c r="N45" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O45" s="6">
         <v>0.54166666666666796</v>
@@ -3244,11 +3236,11 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K46" s="1"/>
       <c r="L46" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="M46" s="1"/>
       <c r="N46" s="10" t="s">
@@ -3465,7 +3457,7 @@
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
@@ -3561,7 +3553,7 @@
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="1"/>
@@ -3645,7 +3637,7 @@
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="10" t="s">
@@ -3666,7 +3658,7 @@
       </c>
       <c r="M55" s="1"/>
       <c r="N55" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O55" s="6">
         <v>0.57638888888889095</v>
@@ -3712,7 +3704,7 @@
       </c>
       <c r="M56" s="1"/>
       <c r="N56" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O56" s="6">
         <v>0.57986111111111305</v>
@@ -3737,11 +3729,11 @@
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="10" t="s">
@@ -3750,15 +3742,15 @@
       <c r="H57" s="18"/>
       <c r="I57" s="1"/>
       <c r="J57" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K57" s="1"/>
       <c r="L57" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M57" s="1"/>
       <c r="N57" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O57" s="6">
         <v>0.58333333333333504</v>
@@ -3783,11 +3775,11 @@
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="10" t="s">
@@ -3921,11 +3913,11 @@
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="10" t="s">
@@ -4013,24 +4005,24 @@
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H63" s="18"/>
       <c r="I63" s="1"/>
       <c r="J63" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K63" s="1"/>
       <c r="L63" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M63" s="1"/>
       <c r="N63" s="10" t="s">
@@ -4059,24 +4051,24 @@
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H64" s="18"/>
       <c r="I64" s="1"/>
       <c r="J64" s="11" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K64" s="1"/>
       <c r="L64" s="11" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="M64" s="1"/>
       <c r="N64" s="10" t="s">
@@ -4197,28 +4189,28 @@
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H67" s="17"/>
       <c r="I67" s="1"/>
       <c r="J67" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K67" s="1"/>
       <c r="L67" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M67" s="1"/>
       <c r="N67" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O67" s="6">
         <v>0.61805555555555802</v>
@@ -4264,7 +4256,7 @@
       </c>
       <c r="M68" s="1"/>
       <c r="N68" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="O68" s="6">
         <v>0.62152777777778001</v>
@@ -4289,11 +4281,11 @@
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="10" t="s">
@@ -4310,7 +4302,7 @@
       </c>
       <c r="M69" s="1"/>
       <c r="N69" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O69" s="6">
         <v>0.625000000000003</v>
@@ -4335,11 +4327,11 @@
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="10" t="s">
@@ -4473,11 +4465,11 @@
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="9" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F73" s="1"/>
       <c r="G73" s="10" t="s">
@@ -4486,11 +4478,11 @@
       <c r="H73" s="18"/>
       <c r="I73" s="1"/>
       <c r="J73" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K73" s="1"/>
       <c r="L73" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M73" s="1"/>
       <c r="N73" s="10" t="s">
@@ -4532,11 +4524,11 @@
       <c r="H74" s="18"/>
       <c r="I74" s="1"/>
       <c r="J74" s="11" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="K74" s="1"/>
       <c r="L74" s="11" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="M74" s="1"/>
       <c r="N74" s="10" t="s">
@@ -4565,7 +4557,7 @@
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="10" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="10" t="s">
@@ -4670,11 +4662,11 @@
       <c r="H77" s="18"/>
       <c r="I77" s="1"/>
       <c r="J77" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K77" s="1"/>
       <c r="L77" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M77" s="1"/>
       <c r="N77" s="10" t="s">
@@ -4770,7 +4762,7 @@
       </c>
       <c r="M79" s="1"/>
       <c r="N79" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O79" s="6">
         <v>0.65972222222222499</v>
@@ -4862,7 +4854,7 @@
       </c>
       <c r="M81" s="1"/>
       <c r="N81" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O81" s="6">
         <v>0.66666666666666996</v>
@@ -4946,11 +4938,11 @@
       <c r="H83" s="18"/>
       <c r="I83" s="1"/>
       <c r="J83" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K83" s="1"/>
       <c r="L83" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M83" s="1"/>
       <c r="N83" s="10" t="s">
@@ -4992,11 +4984,11 @@
       <c r="H84" s="18"/>
       <c r="I84" s="1"/>
       <c r="J84" s="11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K84" s="1"/>
       <c r="L84" s="11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="M84" s="1"/>
       <c r="N84" s="10" t="s">
@@ -5452,11 +5444,11 @@
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K94" s="1"/>
       <c r="L94" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="M94" s="1"/>
       <c r="N94" s="10" t="s">
@@ -5761,7 +5753,7 @@
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="10" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="10" t="s">
@@ -5805,8 +5797,8 @@
       <c r="A102" s="6">
         <v>0.73958333333333703</v>
       </c>
-      <c r="C102" s="11" t="s">
-        <v>17</v>
+      <c r="C102" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="11" t="s">
@@ -5839,7 +5831,7 @@
       <c r="A103" s="6">
         <v>0.74305555555556002</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D103" s="1"/>
@@ -5873,7 +5865,7 @@
       <c r="A104" s="6">
         <v>0.74652777777778201</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D104" s="1"/>
@@ -5887,15 +5879,15 @@
       <c r="H104" s="18"/>
       <c r="I104" s="1"/>
       <c r="J104" s="11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K104" s="1"/>
       <c r="L104" s="11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="M104" s="1"/>
       <c r="N104" s="11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="O104" s="6">
         <v>0.74652777777778201</v>
@@ -5907,8 +5899,8 @@
       <c r="A105" s="6">
         <v>0.750000000000004</v>
       </c>
-      <c r="C105" s="9" t="s">
-        <v>16</v>
+      <c r="C105" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="D105" s="1"/>
       <c r="E105" s="9" t="s">
@@ -5935,12 +5927,12 @@
       <c r="P105" s="1"/>
       <c r="Q105" s="1"/>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="6">
         <v>0.75347222222222598</v>
       </c>
-      <c r="C106" s="10" t="s">
-        <v>10</v>
+      <c r="C106" s="11" t="s">
+        <v>214</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="10" t="s">
@@ -5971,8 +5963,8 @@
       <c r="A107" s="6">
         <v>0.75694444444444897</v>
       </c>
-      <c r="C107" s="10" t="s">
-        <v>13</v>
+      <c r="C107" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D107" s="1"/>
       <c r="E107" s="10" t="s">
@@ -6003,8 +5995,8 @@
       <c r="A108" s="6">
         <v>0.76041666666667096</v>
       </c>
-      <c r="C108" s="11" t="s">
-        <v>11</v>
+      <c r="C108" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="11" t="s">
@@ -6012,7 +6004,7 @@
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
@@ -6136,13 +6128,13 @@
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" s="21" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B114" s="22"/>
       <c r="C114" s="23"/>
       <c r="N114" s="19" t="str">
         <f>A114</f>
-        <v>Last updated: 27.06.2017 14:55</v>
+        <v>Last updated: 28.06.2017 16:20</v>
       </c>
       <c r="O114" s="20"/>
     </row>
@@ -6279,10 +6271,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6298,25 +6290,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -6327,13 +6319,13 @@
         <v>0.40972222222222227</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -6346,13 +6338,13 @@
         <v>0.40972222222222227</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -6365,19 +6357,19 @@
         <v>0.4375</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -6388,19 +6380,19 @@
         <v>0.4375</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -6411,19 +6403,19 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -6434,19 +6426,19 @@
         <v>0.47222222222222227</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="210" x14ac:dyDescent="0.25">
@@ -6457,19 +6449,19 @@
         <v>0.4861111111111111</v>
       </c>
       <c r="C8" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>155</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -6483,16 +6475,16 @@
         <v>7</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6506,16 +6498,16 @@
         <v>5</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -6529,16 +6521,16 @@
         <v>6</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6555,13 +6547,13 @@
         <v>43</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -6572,19 +6564,19 @@
         <v>0.50694444444444442</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6595,19 +6587,19 @@
         <v>0.50694444444444442</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -6621,16 +6613,16 @@
         <v>5</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6644,16 +6636,16 @@
         <v>6</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6664,19 +6656,19 @@
         <v>0.53472222222222221</v>
       </c>
       <c r="C17" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="G17" s="15" t="s">
         <v>155</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6690,16 +6682,16 @@
         <v>7</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6710,19 +6702,19 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6733,19 +6725,19 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -6759,16 +6751,16 @@
         <v>5</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6782,16 +6774,16 @@
         <v>6</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6805,16 +6797,16 @@
         <v>7</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6825,19 +6817,19 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6848,19 +6840,19 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="C25" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="G25" s="15" t="s">
         <v>155</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -6871,19 +6863,19 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -6897,16 +6889,16 @@
         <v>5</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -6920,16 +6912,16 @@
         <v>6</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6943,16 +6935,16 @@
         <v>7</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -6963,19 +6955,19 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -6986,19 +6978,19 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7009,19 +7001,19 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -7032,19 +7024,19 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -7055,19 +7047,19 @@
         <v>0.65972222222222221</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>47</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7081,16 +7073,16 @@
         <v>5</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7104,16 +7096,16 @@
         <v>6</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G36" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7127,16 +7119,16 @@
         <v>7</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7147,19 +7139,19 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7170,19 +7162,19 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>51</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7196,16 +7188,16 @@
         <v>5</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7219,16 +7211,16 @@
         <v>6</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -7239,7 +7231,7 @@
         <v>0.6875</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D42" s="15" t="s">
         <v>37</v>
@@ -7248,10 +7240,10 @@
         <v>45</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7262,7 +7254,7 @@
         <v>0.6875</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>36</v>
@@ -7271,10 +7263,10 @@
         <v>44</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -7285,7 +7277,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>30</v>
@@ -7294,10 +7286,10 @@
         <v>41</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7314,13 +7306,13 @@
         <v>43</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -7340,10 +7332,10 @@
         <v>50</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7363,10 +7355,10 @@
         <v>49</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7377,7 +7369,7 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>25</v>
@@ -7386,10 +7378,10 @@
         <v>32</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7400,7 +7392,7 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D49" s="15" t="s">
         <v>24</v>
@@ -7409,10 +7401,10 @@
         <v>31</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G49" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7432,10 +7424,10 @@
         <v>38</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G50" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -7446,7 +7438,7 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>14</v>
@@ -7455,10 +7447,10 @@
         <v>23</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -7478,10 +7470,10 @@
         <v>35</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -7501,10 +7493,10 @@
         <v>34</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -7512,10 +7504,10 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="B54" s="14">
-        <v>0.74305555555555547</v>
+        <v>0.75694444444444453</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D54" s="15" t="s">
         <v>19</v>
@@ -7524,10 +7516,10 @@
         <v>21</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -7538,7 +7530,7 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D55" s="15" t="s">
         <v>18</v>
@@ -7547,13 +7539,13 @@
         <v>20</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="14">
         <v>0.75</v>
       </c>
@@ -7561,57 +7553,37 @@
         <v>0.76388888888888884</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="14">
-        <v>0.75</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="B57" s="14">
-        <v>0.76388888888888884</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="D57" s="15" t="s">
-        <v>12</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D57" s="15"/>
       <c r="E57" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F57" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="G57" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>0.77083333333333337</v>
-      </c>
-      <c r="B58">
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="C58" t="s">
-        <v>145</v>
-      </c>
-      <c r="E58" s="12" t="s">
         <v>9</v>
       </c>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>